<commit_message>
links back from map to details again, edit map
rotated some booths and stuff, made changes in xls and js array
</commit_message>
<xml_diff>
--- a/full-data-iday14.xlsx
+++ b/full-data-iday14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="1660" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="9200" yWindow="3160" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL 9PM" sheetId="1" r:id="rId1"/>
@@ -3974,7 +3974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
@@ -9271,8 +9271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60:D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -9822,7 +9822,7 @@
         <v>559</v>
       </c>
       <c r="E32" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="13">
@@ -9839,7 +9839,7 @@
         <v>444</v>
       </c>
       <c r="E33" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13">
@@ -9856,7 +9856,7 @@
         <v>354</v>
       </c>
       <c r="E34" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="13">
@@ -9873,7 +9873,7 @@
         <v>258</v>
       </c>
       <c r="E35" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="13">
@@ -9890,7 +9890,7 @@
         <v>160</v>
       </c>
       <c r="E36" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="13">
@@ -10121,14 +10121,14 @@
       <c r="B50" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="128">
         <v>315</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="128">
         <v>223</v>
       </c>
       <c r="E50" s="146">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13">
@@ -10138,14 +10138,14 @@
       <c r="B51" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="128">
         <v>318</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="128">
         <v>314</v>
       </c>
       <c r="E51" s="146">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13">
@@ -10155,14 +10155,14 @@
       <c r="B52" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="128">
         <v>317</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="128">
         <v>411</v>
       </c>
       <c r="E52" s="146">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="13">
@@ -10206,14 +10206,14 @@
       <c r="B55" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="128">
         <v>545</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="128">
         <v>260</v>
       </c>
       <c r="E55" s="146">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="13">
@@ -10223,14 +10223,14 @@
       <c r="B56" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="128">
         <v>545</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="128">
         <v>377</v>
       </c>
       <c r="E56" s="146">
-        <v>90</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="13">
@@ -10247,7 +10247,7 @@
         <v>408</v>
       </c>
       <c r="E57" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="13">
@@ -10264,7 +10264,7 @@
         <v>313</v>
       </c>
       <c r="E58" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="13">
@@ -10281,7 +10281,7 @@
         <v>201</v>
       </c>
       <c r="E59" s="146">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -10291,14 +10291,14 @@
       <c r="B60" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="128">
         <v>825</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="128">
         <v>201</v>
       </c>
       <c r="E60" s="146">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -10308,14 +10308,14 @@
       <c r="B61" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="128">
         <v>825</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="128">
         <v>313</v>
       </c>
       <c r="E61" s="146">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="13">
@@ -10325,14 +10325,14 @@
       <c r="B62" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="128">
         <v>825</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="128">
         <v>405</v>
       </c>
       <c r="E62" s="146">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating booth data in xls
</commit_message>
<xml_diff>
--- a/full-data-iday14.xlsx
+++ b/full-data-iday14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="380" windowWidth="26120" windowHeight="17560" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15040" windowHeight="16060" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FINAL 9PM" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="booth layout prev" sheetId="3" r:id="rId4"/>
     <sheet name="nonfinaldata" sheetId="4" r:id="rId5"/>
     <sheet name="label key" sheetId="6" r:id="rId6"/>
+    <sheet name="updated boothlayout" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'FINAL 9PM'!$F$1:$T$74</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="901">
   <si>
     <t>booth</t>
   </si>
@@ -2178,13 +2179,565 @@
   </si>
   <si>
     <t>the name to display in the company list</t>
+  </si>
+  <si>
+    <t>&lt;svg width="1100" height="2435" viewBox="-10 -800 1000 2225" xmlns="http://www.w3.org/2000/svg" xmlns:svg="http://www.w3.org/2000/svg" xmlns:xlink="http://www.w3.org/1999/xlink"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;!-- Created with SVG-edit - http://svg-edit.googlecode.com/ --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;!-- optimizes using peter collingridge's svg editor/optimiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://petercollingridge.appspot.com/svg-editor --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;style&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   .booth {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   stroke: #000000;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   fill: #ff0000;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   stroke-width: 5;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   }</t>
+  </si>
+  <si>
+    <t>svg {background: lightgrey; }</t>
+  </si>
+  <si>
+    <t>.wall {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   fill-opacity:0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   stroke-linecap: null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   stroke-linejoin: null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   stroke-dasharray: null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   fill: none;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;/style&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;!--</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;g display="inline"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;title&gt;img2&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;image xlink:href="http://i.imgur.com/ArXl22P.png" id="svg_1" height="1248" width="953" y="185" x="8"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;/g&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;title&gt;newimg&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;image xlink:href="http://i.imgur.com/HphIdr8.png" id="svg_2" height="2251" width="964" y="-818" x="5"/&gt;</t>
+  </si>
+  <si>
+    <t>--&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;title&gt;booths&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;g id="svg_19"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;rect</t>
+  </si>
+  <si>
+    <t>svg_57</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>booth/&gt;</t>
+  </si>
+  <si>
+    <t>svg_80</t>
+  </si>
+  <si>
+    <t>svg_81</t>
+  </si>
+  <si>
+    <t>svg_82</t>
+  </si>
+  <si>
+    <t>svg_83</t>
+  </si>
+  <si>
+    <t>svg_84</t>
+  </si>
+  <si>
+    <t>transform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate(-90 59.99997329711909,-376.33334350585943) </t>
+  </si>
+  <si>
+    <t>svg_85</t>
+  </si>
+  <si>
+    <t>24/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate(-90 51.999973297119034,-651.0000000000001) </t>
+  </si>
+  <si>
+    <t>svg_86</t>
+  </si>
+  <si>
+    <t>581/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate(90 609.3333129882812,-104.33332061767577) </t>
+  </si>
+  <si>
+    <t>svg_87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate(-39.55965042114258 73.33332061767582,-194.9999847412109) </t>
+  </si>
+  <si>
+    <t>svg_88</t>
+  </si>
+  <si>
+    <t>56/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate(42.51044845581055 83.99998474121094,13.000009536743162) </t>
+  </si>
+  <si>
+    <t>svg_3/&gt;</t>
+  </si>
+  <si>
+    <t>svg_4/&gt;</t>
+  </si>
+  <si>
+    <t>svg_5/&gt;</t>
+  </si>
+  <si>
+    <t>svg_6/&gt;</t>
+  </si>
+  <si>
+    <t>svg_7/&gt;</t>
+  </si>
+  <si>
+    <t>svg_8/&gt;</t>
+  </si>
+  <si>
+    <t>svg_9/&gt;</t>
+  </si>
+  <si>
+    <t>svg_10/&gt;</t>
+  </si>
+  <si>
+    <t>svg_11/&gt;</t>
+  </si>
+  <si>
+    <t>svg_12/&gt;</t>
+  </si>
+  <si>
+    <t>svg_13/&gt;</t>
+  </si>
+  <si>
+    <t>svg_14/&gt;</t>
+  </si>
+  <si>
+    <t>svg_15/&gt;</t>
+  </si>
+  <si>
+    <t>svg_16/&gt;</t>
+  </si>
+  <si>
+    <t>svg_17/&gt;</t>
+  </si>
+  <si>
+    <t>svg_18/&gt;</t>
+  </si>
+  <si>
+    <t>svg_20/&gt;</t>
+  </si>
+  <si>
+    <t>svg_21/&gt;</t>
+  </si>
+  <si>
+    <t>svg_22/&gt;</t>
+  </si>
+  <si>
+    <t>svg_23/&gt;</t>
+  </si>
+  <si>
+    <t>svg_24/&gt;</t>
+  </si>
+  <si>
+    <t>svg_25/&gt;</t>
+  </si>
+  <si>
+    <t>svg_26/&gt;</t>
+  </si>
+  <si>
+    <t>svg_27/&gt;</t>
+  </si>
+  <si>
+    <t>svg_28/&gt;</t>
+  </si>
+  <si>
+    <t>svg_29/&gt;</t>
+  </si>
+  <si>
+    <t>svg_30/&gt;</t>
+  </si>
+  <si>
+    <t>svg_31/&gt;</t>
+  </si>
+  <si>
+    <t>svg_32/&gt;</t>
+  </si>
+  <si>
+    <t>svg_33</t>
+  </si>
+  <si>
+    <t>matrix(0.7008790586895676,0.5186515302772782,-0.5186515302772782,0.7008790586895676,196.13764103827577,-306.0634716546593) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_34/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matrix(0.531614842633715,-0.6910980566171975,0.6910980566171975,0.531614842633715,-42.99335129261749,271.0982186362347) </t>
+  </si>
+  <si>
+    <t>svg_35/&gt;</t>
+  </si>
+  <si>
+    <t>svg_36/&gt;</t>
+  </si>
+  <si>
+    <t>svg_37/&gt;</t>
+  </si>
+  <si>
+    <t>svg_38</t>
+  </si>
+  <si>
+    <t>matrix(0.638933169263332,-0.5932918927337969,0.5932918927337969,0.638933169263332,-225.76544504101662,968.0253084882027) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_39/&gt;</t>
+  </si>
+  <si>
+    <t>svg_40/&gt;</t>
+  </si>
+  <si>
+    <t>svg_41/&gt;</t>
+  </si>
+  <si>
+    <t>svg_42/&gt;</t>
+  </si>
+  <si>
+    <t>svg_43/&gt;</t>
+  </si>
+  <si>
+    <t>svg_44/&gt;</t>
+  </si>
+  <si>
+    <t>svg_45/&gt;</t>
+  </si>
+  <si>
+    <t>svg_46/&gt;</t>
+  </si>
+  <si>
+    <t>svg_47/&gt;</t>
+  </si>
+  <si>
+    <t>svg_48/&gt;</t>
+  </si>
+  <si>
+    <t>svg_49/&gt;</t>
+  </si>
+  <si>
+    <t>svg_50</t>
+  </si>
+  <si>
+    <t>matrix(4.6440852291236576e-7,-0.8719121886797552,0.8719121886797552,4.6440852291236576e-7,-835.734608805689,1472.0783421106814) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_51</t>
+  </si>
+  <si>
+    <t>matrix(0.7127737068708423,-0.5,0.5021797562249352,0.7127737068708423,-497.63622158381645,500.38574908686286) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_52</t>
+  </si>
+  <si>
+    <t>matrix(0.03287766790076221,0.8712921001145045,-0.9,0,1770,433) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_53/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matrix(0,0.9,-0.9,0.03287766790076221,1531.4962704153527,710.3756954396183) </t>
+  </si>
+  <si>
+    <t>svg_54</t>
+  </si>
+  <si>
+    <t>matrix(-0.1,-0.9,0.9,-0.1,-628,1712) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_55</t>
+  </si>
+  <si>
+    <t>matrix(0.5,0.7,-0.7,0.5,1075,505) /&gt;</t>
+  </si>
+  <si>
+    <t>svg_56</t>
+  </si>
+  <si>
+    <t>matrix(0.5,-0,0.6,0.6,-640,1092) /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;path</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>m12 904l0-717 946-1 0 719 -179-1 13-30 -114 0 15 31 -6810 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0z</t>
+  </si>
+  <si>
+    <t>svg_58/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;line</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>svg_59/&gt;</t>
+  </si>
+  <si>
+    <t>svg_60/&gt;</t>
+  </si>
+  <si>
+    <t>svg_61/&gt;</t>
+  </si>
+  <si>
+    <t>svg_62/&gt;</t>
+  </si>
+  <si>
+    <t>svg_63/&gt;</t>
+  </si>
+  <si>
+    <t>svg_64/&gt;</t>
+  </si>
+  <si>
+    <t>svg_65/&gt;</t>
+  </si>
+  <si>
+    <t>svg_66/&gt;</t>
+  </si>
+  <si>
+    <t>svg_67/&gt;</t>
+  </si>
+  <si>
+    <t>svg_68/&gt;</t>
+  </si>
+  <si>
+    <t>svg_69/&gt;</t>
+  </si>
+  <si>
+    <t>svg_70/&gt;</t>
+  </si>
+  <si>
+    <t>svg_71/&gt;</t>
+  </si>
+  <si>
+    <t>svg_72/&gt;</t>
+  </si>
+  <si>
+    <t>svg_73/&gt;</t>
+  </si>
+  <si>
+    <t>svg_74/&gt;</t>
+  </si>
+  <si>
+    <t>svg_75/&gt;</t>
+  </si>
+  <si>
+    <t>svg_76/&gt;</t>
+  </si>
+  <si>
+    <t>m401 1073l-193-1 0 354 589 0 0-359 -296-1 30 40 -163-1 33-32 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0z</t>
+  </si>
+  <si>
+    <t>svg_77/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;text</t>
+  </si>
+  <si>
+    <t>stroke</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>stroke-width</t>
+  </si>
+  <si>
+    <t>svg_78</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>font-family</t>
+  </si>
+  <si>
+    <t>serif</t>
+  </si>
+  <si>
+    <t>text-anchor</t>
+  </si>
+  <si>
+    <t>middle</t>
+  </si>
+  <si>
+    <t>xml:space</t>
+  </si>
+  <si>
+    <t>preserve</t>
+  </si>
+  <si>
+    <t>matrix(0.9757868429625915,0,0,0.8719121886798789,-23.078713037476177,183.8957192263419) &gt;Northshore</t>
+  </si>
+  <si>
+    <t>Room&lt;/text&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matrix(0.9757868429625913,0,0,0.8719121886798789,161.46109724516543,184.55850812316598) </t>
+  </si>
+  <si>
+    <t>svg_79&gt;Lakeshore</t>
+  </si>
+  <si>
+    <t>svg_90</t>
+  </si>
+  <si>
+    <t>225/&gt;</t>
+  </si>
+  <si>
+    <t>svg_91</t>
+  </si>
+  <si>
+    <t>288/&gt;</t>
+  </si>
+  <si>
+    <t>svg_93</t>
+  </si>
+  <si>
+    <t>220/&gt;</t>
+  </si>
+  <si>
+    <t>svg_94</t>
+  </si>
+  <si>
+    <t>640/&gt;</t>
+  </si>
+  <si>
+    <t>svg_95</t>
+  </si>
+  <si>
+    <t>654/&gt;</t>
+  </si>
+  <si>
+    <t>svg_96</t>
+  </si>
+  <si>
+    <t>649/&gt;</t>
+  </si>
+  <si>
+    <t>svg_97</t>
+  </si>
+  <si>
+    <t>427/&gt;</t>
+  </si>
+  <si>
+    <t>svg_98</t>
+  </si>
+  <si>
+    <t>428/&gt;</t>
+  </si>
+  <si>
+    <t>svg_99</t>
+  </si>
+  <si>
+    <t>22/&gt;</t>
+  </si>
+  <si>
+    <t>svg_92/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;/g&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/svg&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2348,8 +2901,15 @@
       <sz val="14"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2389,6 +2949,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3008,7 +3574,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3198,8 +3764,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3717,8 +4301,13 @@
     <xf numFmtId="0" fontId="27" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -3812,6 +4401,15 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -3905,6 +4503,15 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Output" xfId="70" builtinId="21"/>
@@ -19578,7 +20185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -19731,4 +20338,2750 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AB155"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15">
+      <c r="E40" t="s">
+        <v>746</v>
+      </c>
+      <c r="F40" t="s">
+        <v>750</v>
+      </c>
+      <c r="G40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="193" t="s">
+        <v>2</v>
+      </c>
+      <c r="I40" s="193" t="s">
+        <v>174</v>
+      </c>
+      <c r="J40" s="193" t="s">
+        <v>175</v>
+      </c>
+      <c r="K40" s="193" t="s">
+        <v>749</v>
+      </c>
+      <c r="L40" s="193" t="s">
+        <v>748</v>
+      </c>
+      <c r="M40" s="194" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="H41" s="147" t="s">
+        <v>747</v>
+      </c>
+      <c r="I41" s="147">
+        <v>63</v>
+      </c>
+      <c r="J41" s="147">
+        <v>-771</v>
+      </c>
+      <c r="K41" s="147">
+        <v>56</v>
+      </c>
+      <c r="L41" s="147">
+        <v>21</v>
+      </c>
+      <c r="P41" t="s">
+        <v>750</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="H42" s="147" t="s">
+        <v>752</v>
+      </c>
+      <c r="I42" s="147">
+        <v>293</v>
+      </c>
+      <c r="J42" s="147">
+        <v>-766</v>
+      </c>
+      <c r="K42" s="147">
+        <v>56</v>
+      </c>
+      <c r="L42" s="147">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="H43" s="147" t="s">
+        <v>753</v>
+      </c>
+      <c r="I43" s="147">
+        <v>59</v>
+      </c>
+      <c r="J43" s="147">
+        <v>-534</v>
+      </c>
+      <c r="K43" s="147">
+        <v>56</v>
+      </c>
+      <c r="L43" s="147">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="H44" s="147" t="s">
+        <v>754</v>
+      </c>
+      <c r="I44" s="147">
+        <v>539</v>
+      </c>
+      <c r="J44" s="147">
+        <v>96</v>
+      </c>
+      <c r="K44" s="147">
+        <v>56</v>
+      </c>
+      <c r="L44" s="147">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="H45" s="147" t="s">
+        <v>755</v>
+      </c>
+      <c r="I45" s="147">
+        <v>669</v>
+      </c>
+      <c r="J45" s="147">
+        <v>77</v>
+      </c>
+      <c r="K45" s="147">
+        <v>56</v>
+      </c>
+      <c r="L45" s="147">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="H46" s="147" t="s">
+        <v>756</v>
+      </c>
+      <c r="I46" s="147">
+        <v>32</v>
+      </c>
+      <c r="J46" s="147">
+        <v>-387</v>
+      </c>
+      <c r="K46" s="147">
+        <v>56</v>
+      </c>
+      <c r="L46" s="147">
+        <v>21</v>
+      </c>
+      <c r="M46" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="H47" s="147" t="s">
+        <v>759</v>
+      </c>
+      <c r="I47" s="147" t="s">
+        <v>760</v>
+      </c>
+      <c r="J47" s="147">
+        <v>-662</v>
+      </c>
+      <c r="K47" s="147">
+        <v>56</v>
+      </c>
+      <c r="L47" s="147">
+        <v>21</v>
+      </c>
+      <c r="M47" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="H48" s="147" t="s">
+        <v>762</v>
+      </c>
+      <c r="I48" s="147" t="s">
+        <v>763</v>
+      </c>
+      <c r="J48" s="147">
+        <v>-115</v>
+      </c>
+      <c r="K48" s="147">
+        <v>56</v>
+      </c>
+      <c r="L48" s="147">
+        <v>21</v>
+      </c>
+      <c r="M48" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="49" spans="8:13">
+      <c r="H49" s="147" t="s">
+        <v>765</v>
+      </c>
+      <c r="I49" s="147">
+        <v>45</v>
+      </c>
+      <c r="J49" s="147">
+        <v>-206</v>
+      </c>
+      <c r="K49" s="147">
+        <v>56</v>
+      </c>
+      <c r="L49" s="147">
+        <v>21</v>
+      </c>
+      <c r="M49" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="50" spans="8:13">
+      <c r="H50" s="147" t="s">
+        <v>767</v>
+      </c>
+      <c r="I50" s="147" t="s">
+        <v>768</v>
+      </c>
+      <c r="J50" s="147">
+        <v>2</v>
+      </c>
+      <c r="K50" s="147">
+        <v>56</v>
+      </c>
+      <c r="L50" s="147">
+        <v>21</v>
+      </c>
+      <c r="M50" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="51" spans="8:13">
+      <c r="H51" s="147" t="s">
+        <v>770</v>
+      </c>
+      <c r="I51" s="147">
+        <v>41</v>
+      </c>
+      <c r="J51" s="147">
+        <v>332</v>
+      </c>
+      <c r="K51" s="147">
+        <v>21</v>
+      </c>
+      <c r="L51" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="8:13">
+      <c r="H52" s="147" t="s">
+        <v>771</v>
+      </c>
+      <c r="I52" s="147">
+        <v>40</v>
+      </c>
+      <c r="J52" s="147">
+        <v>425</v>
+      </c>
+      <c r="K52" s="147">
+        <v>21</v>
+      </c>
+      <c r="L52" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="8:13">
+      <c r="H53" s="147" t="s">
+        <v>772</v>
+      </c>
+      <c r="I53" s="147">
+        <v>43</v>
+      </c>
+      <c r="J53" s="147">
+        <v>513</v>
+      </c>
+      <c r="K53" s="147">
+        <v>18</v>
+      </c>
+      <c r="L53" s="147">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="8:13">
+      <c r="H54" s="147" t="s">
+        <v>773</v>
+      </c>
+      <c r="I54" s="147">
+        <v>43</v>
+      </c>
+      <c r="J54" s="147">
+        <v>585</v>
+      </c>
+      <c r="K54" s="147">
+        <v>18</v>
+      </c>
+      <c r="L54" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="8:13">
+      <c r="H55" s="147" t="s">
+        <v>774</v>
+      </c>
+      <c r="I55" s="147">
+        <v>39</v>
+      </c>
+      <c r="J55" s="147">
+        <v>691</v>
+      </c>
+      <c r="K55" s="147">
+        <v>20</v>
+      </c>
+      <c r="L55" s="147">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="8:13">
+      <c r="H56" s="147" t="s">
+        <v>775</v>
+      </c>
+      <c r="I56" s="147">
+        <v>238</v>
+      </c>
+      <c r="J56" s="147">
+        <v>382</v>
+      </c>
+      <c r="K56" s="147">
+        <v>22</v>
+      </c>
+      <c r="L56" s="147">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="8:13">
+      <c r="H57" s="147" t="s">
+        <v>776</v>
+      </c>
+      <c r="I57" s="147">
+        <v>281</v>
+      </c>
+      <c r="J57" s="147">
+        <v>378</v>
+      </c>
+      <c r="K57" s="147">
+        <v>27</v>
+      </c>
+      <c r="L57" s="147">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="8:13">
+      <c r="H58" s="147" t="s">
+        <v>777</v>
+      </c>
+      <c r="I58" s="147">
+        <v>237</v>
+      </c>
+      <c r="J58" s="147">
+        <v>456</v>
+      </c>
+      <c r="K58" s="147">
+        <v>21</v>
+      </c>
+      <c r="L58" s="147">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="8:13">
+      <c r="H59" s="147" t="s">
+        <v>778</v>
+      </c>
+      <c r="I59" s="147">
+        <v>284</v>
+      </c>
+      <c r="J59" s="147">
+        <v>458</v>
+      </c>
+      <c r="K59" s="147">
+        <v>24</v>
+      </c>
+      <c r="L59" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="8:13">
+      <c r="H60" s="147" t="s">
+        <v>779</v>
+      </c>
+      <c r="I60" s="147">
+        <v>235</v>
+      </c>
+      <c r="J60" s="147">
+        <v>541</v>
+      </c>
+      <c r="K60" s="147">
+        <v>22</v>
+      </c>
+      <c r="L60" s="147">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="8:13">
+      <c r="H61" s="147" t="s">
+        <v>780</v>
+      </c>
+      <c r="I61" s="147">
+        <v>283</v>
+      </c>
+      <c r="J61" s="147">
+        <v>542</v>
+      </c>
+      <c r="K61" s="147">
+        <v>27</v>
+      </c>
+      <c r="L61" s="147">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="8:13">
+      <c r="H62" s="147" t="s">
+        <v>781</v>
+      </c>
+      <c r="I62" s="147">
+        <v>284</v>
+      </c>
+      <c r="J62" s="147">
+        <v>217</v>
+      </c>
+      <c r="K62" s="147">
+        <v>65</v>
+      </c>
+      <c r="L62" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="8:13">
+      <c r="H63" s="147" t="s">
+        <v>782</v>
+      </c>
+      <c r="I63" s="147">
+        <v>463</v>
+      </c>
+      <c r="J63" s="147">
+        <v>214</v>
+      </c>
+      <c r="K63" s="147">
+        <v>54</v>
+      </c>
+      <c r="L63" s="147">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="8:13">
+      <c r="H64" s="147" t="s">
+        <v>783</v>
+      </c>
+      <c r="I64" s="147">
+        <v>576</v>
+      </c>
+      <c r="J64" s="147">
+        <v>216</v>
+      </c>
+      <c r="K64" s="147">
+        <v>56</v>
+      </c>
+      <c r="L64" s="147">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="8:12">
+      <c r="H65" s="147" t="s">
+        <v>784</v>
+      </c>
+      <c r="I65" s="147">
+        <v>678</v>
+      </c>
+      <c r="J65" s="147">
+        <v>359</v>
+      </c>
+      <c r="K65" s="147">
+        <v>17</v>
+      </c>
+      <c r="L65" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="8:12">
+      <c r="H66" s="147" t="s">
+        <v>785</v>
+      </c>
+      <c r="I66" s="147">
+        <v>727</v>
+      </c>
+      <c r="J66" s="147">
+        <v>360</v>
+      </c>
+      <c r="K66" s="147">
+        <v>17</v>
+      </c>
+      <c r="L66" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="8:12">
+      <c r="H67" s="147" t="s">
+        <v>786</v>
+      </c>
+      <c r="I67" s="147">
+        <v>678</v>
+      </c>
+      <c r="J67" s="147">
+        <v>457</v>
+      </c>
+      <c r="K67" s="147">
+        <v>17</v>
+      </c>
+      <c r="L67" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="8:12">
+      <c r="H68" s="147" t="s">
+        <v>787</v>
+      </c>
+      <c r="I68" s="147">
+        <v>727</v>
+      </c>
+      <c r="J68" s="147">
+        <v>456</v>
+      </c>
+      <c r="K68" s="147">
+        <v>17</v>
+      </c>
+      <c r="L68" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="8:12">
+      <c r="H69" s="147" t="s">
+        <v>788</v>
+      </c>
+      <c r="I69" s="147">
+        <v>680</v>
+      </c>
+      <c r="J69" s="147">
+        <v>540</v>
+      </c>
+      <c r="K69" s="147">
+        <v>17</v>
+      </c>
+      <c r="L69" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="8:12">
+      <c r="H70" s="147" t="s">
+        <v>789</v>
+      </c>
+      <c r="I70" s="147">
+        <v>725</v>
+      </c>
+      <c r="J70" s="147">
+        <v>537</v>
+      </c>
+      <c r="K70" s="147">
+        <v>17</v>
+      </c>
+      <c r="L70" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="8:12">
+      <c r="H71" s="147" t="s">
+        <v>790</v>
+      </c>
+      <c r="I71" s="147">
+        <v>908</v>
+      </c>
+      <c r="J71" s="147">
+        <v>324</v>
+      </c>
+      <c r="K71" s="147">
+        <v>17</v>
+      </c>
+      <c r="L71" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="8:12">
+      <c r="H72" s="147" t="s">
+        <v>791</v>
+      </c>
+      <c r="I72" s="147">
+        <v>909</v>
+      </c>
+      <c r="J72" s="147">
+        <v>409</v>
+      </c>
+      <c r="K72" s="147">
+        <v>17</v>
+      </c>
+      <c r="L72" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="8:12">
+      <c r="H73" s="147" t="s">
+        <v>792</v>
+      </c>
+      <c r="I73" s="147">
+        <v>909</v>
+      </c>
+      <c r="J73" s="147">
+        <v>493</v>
+      </c>
+      <c r="K73" s="147">
+        <v>17</v>
+      </c>
+      <c r="L73" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="8:12">
+      <c r="H74" s="147" t="s">
+        <v>793</v>
+      </c>
+      <c r="I74" s="147">
+        <v>908</v>
+      </c>
+      <c r="J74" s="147">
+        <v>571</v>
+      </c>
+      <c r="K74" s="147">
+        <v>17</v>
+      </c>
+      <c r="L74" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="8:12">
+      <c r="H75" s="147" t="s">
+        <v>794</v>
+      </c>
+      <c r="I75" s="147">
+        <v>907</v>
+      </c>
+      <c r="J75" s="147">
+        <v>671</v>
+      </c>
+      <c r="K75" s="147">
+        <v>17</v>
+      </c>
+      <c r="L75" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="8:12">
+      <c r="H76" s="147" t="s">
+        <v>795</v>
+      </c>
+      <c r="I76" s="147">
+        <v>433</v>
+      </c>
+      <c r="J76" s="147">
+        <v>411</v>
+      </c>
+      <c r="K76" s="147">
+        <v>17</v>
+      </c>
+      <c r="L76" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="8:12">
+      <c r="H77" s="147" t="s">
+        <v>796</v>
+      </c>
+      <c r="I77" s="147">
+        <v>482</v>
+      </c>
+      <c r="J77" s="147">
+        <v>411</v>
+      </c>
+      <c r="K77" s="147">
+        <v>17</v>
+      </c>
+      <c r="L77" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="8:12">
+      <c r="H78" s="147" t="s">
+        <v>797</v>
+      </c>
+      <c r="I78" s="147">
+        <v>432</v>
+      </c>
+      <c r="J78" s="147">
+        <v>511</v>
+      </c>
+      <c r="K78" s="147">
+        <v>17</v>
+      </c>
+      <c r="L78" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="8:12">
+      <c r="H79" s="147" t="s">
+        <v>798</v>
+      </c>
+      <c r="I79" s="147">
+        <v>481</v>
+      </c>
+      <c r="J79" s="147">
+        <v>513</v>
+      </c>
+      <c r="K79" s="147">
+        <v>17</v>
+      </c>
+      <c r="L79" s="147">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="8:12">
+      <c r="H80" s="147"/>
+      <c r="I80" s="147"/>
+      <c r="J80" s="147"/>
+      <c r="K80" s="147"/>
+      <c r="L80" s="147"/>
+    </row>
+    <row r="81" spans="8:13">
+      <c r="H81" s="147" t="s">
+        <v>799</v>
+      </c>
+      <c r="I81" s="147">
+        <v>956</v>
+      </c>
+      <c r="J81" s="147">
+        <v>39</v>
+      </c>
+      <c r="K81" s="147">
+        <v>74</v>
+      </c>
+      <c r="L81" s="147">
+        <v>21</v>
+      </c>
+      <c r="M81" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="82" spans="8:13">
+      <c r="H82" s="147" t="s">
+        <v>801</v>
+      </c>
+      <c r="I82" s="147">
+        <v>52</v>
+      </c>
+      <c r="J82" s="147">
+        <v>80</v>
+      </c>
+      <c r="K82" s="147">
+        <v>74</v>
+      </c>
+      <c r="L82" s="147">
+        <v>21</v>
+      </c>
+      <c r="M82" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="83" spans="8:13">
+      <c r="H83" s="147"/>
+      <c r="I83" s="147"/>
+      <c r="J83" s="147"/>
+      <c r="K83" s="147"/>
+      <c r="L83" s="147"/>
+    </row>
+    <row r="84" spans="8:13">
+      <c r="H84" s="147" t="s">
+        <v>803</v>
+      </c>
+      <c r="I84" s="147">
+        <v>65</v>
+      </c>
+      <c r="J84" s="147">
+        <v>839</v>
+      </c>
+      <c r="K84" s="147">
+        <v>65</v>
+      </c>
+      <c r="L84" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="8:13">
+      <c r="H85" s="147" t="s">
+        <v>804</v>
+      </c>
+      <c r="I85" s="147">
+        <v>269</v>
+      </c>
+      <c r="J85" s="147">
+        <v>838</v>
+      </c>
+      <c r="K85" s="147">
+        <v>65</v>
+      </c>
+      <c r="L85" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="8:13">
+      <c r="H86" s="147" t="s">
+        <v>805</v>
+      </c>
+      <c r="I86" s="147">
+        <v>559</v>
+      </c>
+      <c r="J86" s="147">
+        <v>857</v>
+      </c>
+      <c r="K86" s="147">
+        <v>65</v>
+      </c>
+      <c r="L86" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="8:13">
+      <c r="H87" s="147" t="s">
+        <v>806</v>
+      </c>
+      <c r="I87" s="147">
+        <v>988</v>
+      </c>
+      <c r="J87" s="147">
+        <v>754</v>
+      </c>
+      <c r="K87" s="147">
+        <v>74</v>
+      </c>
+      <c r="L87" s="147">
+        <v>21</v>
+      </c>
+      <c r="M87" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="88" spans="8:13">
+      <c r="H88" s="147"/>
+      <c r="I88" s="147"/>
+      <c r="J88" s="147"/>
+      <c r="K88" s="147"/>
+      <c r="L88" s="147"/>
+    </row>
+    <row r="89" spans="8:13">
+      <c r="H89" s="147" t="s">
+        <v>808</v>
+      </c>
+      <c r="I89" s="147">
+        <v>248</v>
+      </c>
+      <c r="J89" s="147">
+        <v>947</v>
+      </c>
+      <c r="K89" s="147">
+        <v>65</v>
+      </c>
+      <c r="L89" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="8:13">
+      <c r="H90" s="147" t="s">
+        <v>809</v>
+      </c>
+      <c r="I90" s="147">
+        <v>23</v>
+      </c>
+      <c r="J90" s="147">
+        <v>923</v>
+      </c>
+      <c r="K90" s="147">
+        <v>65</v>
+      </c>
+      <c r="L90" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="8:13">
+      <c r="H91" s="147" t="s">
+        <v>810</v>
+      </c>
+      <c r="I91" s="147">
+        <v>595</v>
+      </c>
+      <c r="J91" s="147">
+        <v>921</v>
+      </c>
+      <c r="K91" s="147">
+        <v>65</v>
+      </c>
+      <c r="L91" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="8:13">
+      <c r="H92" s="147" t="s">
+        <v>811</v>
+      </c>
+      <c r="I92" s="147">
+        <v>183</v>
+      </c>
+      <c r="J92" s="147">
+        <v>1032</v>
+      </c>
+      <c r="K92" s="147">
+        <v>65</v>
+      </c>
+      <c r="L92" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="8:13">
+      <c r="H93" s="147" t="s">
+        <v>812</v>
+      </c>
+      <c r="I93" s="147">
+        <v>283</v>
+      </c>
+      <c r="J93" s="147">
+        <v>1035</v>
+      </c>
+      <c r="K93" s="147">
+        <v>65</v>
+      </c>
+      <c r="L93" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="8:13">
+      <c r="H94" s="147" t="s">
+        <v>813</v>
+      </c>
+      <c r="I94" s="147">
+        <v>514</v>
+      </c>
+      <c r="J94" s="147">
+        <v>1036</v>
+      </c>
+      <c r="K94" s="147">
+        <v>65</v>
+      </c>
+      <c r="L94" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="8:13">
+      <c r="H95" s="147" t="s">
+        <v>814</v>
+      </c>
+      <c r="I95" s="147">
+        <v>625</v>
+      </c>
+      <c r="J95" s="147">
+        <v>1036</v>
+      </c>
+      <c r="K95" s="147">
+        <v>65</v>
+      </c>
+      <c r="L95" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="8:13">
+      <c r="H96" s="147" t="s">
+        <v>815</v>
+      </c>
+      <c r="I96" s="147">
+        <v>740</v>
+      </c>
+      <c r="J96" s="147">
+        <v>1038</v>
+      </c>
+      <c r="K96" s="147">
+        <v>65</v>
+      </c>
+      <c r="L96" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17">
+      <c r="H97" s="147" t="s">
+        <v>816</v>
+      </c>
+      <c r="I97" s="147">
+        <v>851</v>
+      </c>
+      <c r="J97" s="147">
+        <v>918</v>
+      </c>
+      <c r="K97" s="147">
+        <v>65</v>
+      </c>
+      <c r="L97" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17">
+      <c r="H98" s="147" t="s">
+        <v>817</v>
+      </c>
+      <c r="I98" s="147">
+        <v>845</v>
+      </c>
+      <c r="J98" s="147">
+        <v>1036</v>
+      </c>
+      <c r="K98" s="147">
+        <v>65</v>
+      </c>
+      <c r="L98" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17">
+      <c r="H99" s="147" t="s">
+        <v>818</v>
+      </c>
+      <c r="I99" s="147">
+        <v>656</v>
+      </c>
+      <c r="J99" s="147">
+        <v>1099</v>
+      </c>
+      <c r="K99" s="147">
+        <v>65</v>
+      </c>
+      <c r="L99" s="147">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17">
+      <c r="H100" s="147"/>
+      <c r="I100" s="147"/>
+      <c r="J100" s="147"/>
+      <c r="K100" s="147"/>
+      <c r="L100" s="147"/>
+    </row>
+    <row r="101" spans="1:17">
+      <c r="H101" s="147" t="s">
+        <v>819</v>
+      </c>
+      <c r="I101" s="147">
+        <v>233</v>
+      </c>
+      <c r="J101" s="147">
+        <v>1213</v>
+      </c>
+      <c r="K101" s="147">
+        <v>74</v>
+      </c>
+      <c r="L101" s="147">
+        <v>21</v>
+      </c>
+      <c r="M101" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17">
+      <c r="H102" s="147" t="s">
+        <v>821</v>
+      </c>
+      <c r="I102" s="147">
+        <v>257</v>
+      </c>
+      <c r="J102" s="147">
+        <v>1051</v>
+      </c>
+      <c r="K102" s="147">
+        <v>74</v>
+      </c>
+      <c r="L102" s="147">
+        <v>21</v>
+      </c>
+      <c r="M102" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17">
+      <c r="H103" s="147" t="s">
+        <v>823</v>
+      </c>
+      <c r="I103" s="147">
+        <v>829</v>
+      </c>
+      <c r="J103" s="147">
+        <v>1169</v>
+      </c>
+      <c r="K103" s="147">
+        <v>74</v>
+      </c>
+      <c r="L103" s="147">
+        <v>21</v>
+      </c>
+      <c r="M103" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17">
+      <c r="H104" s="147" t="s">
+        <v>825</v>
+      </c>
+      <c r="I104" s="147">
+        <v>527</v>
+      </c>
+      <c r="J104" s="147">
+        <v>1186</v>
+      </c>
+      <c r="K104" s="147">
+        <v>74</v>
+      </c>
+      <c r="L104" s="147">
+        <v>21</v>
+      </c>
+      <c r="M104" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17">
+      <c r="H105" s="147" t="s">
+        <v>827</v>
+      </c>
+      <c r="I105" s="147">
+        <v>460</v>
+      </c>
+      <c r="J105" s="147">
+        <v>1221</v>
+      </c>
+      <c r="K105" s="147">
+        <v>74</v>
+      </c>
+      <c r="L105" s="147">
+        <v>21</v>
+      </c>
+      <c r="M105" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17">
+      <c r="H106" s="147" t="s">
+        <v>829</v>
+      </c>
+      <c r="I106" s="147">
+        <v>243</v>
+      </c>
+      <c r="J106" s="147">
+        <v>1335</v>
+      </c>
+      <c r="K106" s="147">
+        <v>74</v>
+      </c>
+      <c r="L106" s="147">
+        <v>21</v>
+      </c>
+      <c r="M106" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17">
+      <c r="H107" s="147" t="s">
+        <v>831</v>
+      </c>
+      <c r="I107" s="147">
+        <v>799</v>
+      </c>
+      <c r="J107" s="147">
+        <v>1340</v>
+      </c>
+      <c r="K107" s="147">
+        <v>74</v>
+      </c>
+      <c r="L107" s="147">
+        <v>21</v>
+      </c>
+      <c r="M107" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17">
+      <c r="A108" s="195"/>
+      <c r="B108" s="195"/>
+      <c r="C108" s="195"/>
+      <c r="D108" s="195"/>
+      <c r="E108" s="195"/>
+      <c r="F108" s="195"/>
+      <c r="G108" s="195"/>
+      <c r="H108" s="195"/>
+      <c r="I108" s="195"/>
+      <c r="J108" s="195"/>
+      <c r="K108" s="195"/>
+      <c r="L108" s="195"/>
+      <c r="M108" s="195"/>
+      <c r="N108" s="195"/>
+      <c r="O108" s="195"/>
+      <c r="P108" s="195"/>
+      <c r="Q108" s="195"/>
+    </row>
+    <row r="109" spans="1:17">
+      <c r="E109" t="s">
+        <v>833</v>
+      </c>
+      <c r="F109" t="s">
+        <v>750</v>
+      </c>
+      <c r="G109" t="s">
+        <v>834</v>
+      </c>
+      <c r="H109" t="s">
+        <v>835</v>
+      </c>
+      <c r="I109" t="s">
+        <v>836</v>
+      </c>
+      <c r="J109" t="s">
+        <v>2</v>
+      </c>
+      <c r="K109" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17">
+      <c r="E111" t="s">
+        <v>838</v>
+      </c>
+      <c r="F111" t="s">
+        <v>750</v>
+      </c>
+      <c r="G111" t="s">
+        <v>834</v>
+      </c>
+      <c r="H111" t="s">
+        <v>839</v>
+      </c>
+      <c r="I111">
+        <v>202</v>
+      </c>
+      <c r="J111" t="s">
+        <v>840</v>
+      </c>
+      <c r="K111">
+        <v>218</v>
+      </c>
+      <c r="L111" t="s">
+        <v>841</v>
+      </c>
+      <c r="M111">
+        <v>178</v>
+      </c>
+      <c r="N111" t="s">
+        <v>842</v>
+      </c>
+      <c r="O111">
+        <v>186</v>
+      </c>
+      <c r="P111" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17">
+      <c r="E112" t="s">
+        <v>838</v>
+      </c>
+      <c r="F112" t="s">
+        <v>750</v>
+      </c>
+      <c r="G112" t="s">
+        <v>834</v>
+      </c>
+      <c r="H112" t="s">
+        <v>839</v>
+      </c>
+      <c r="I112">
+        <v>420</v>
+      </c>
+      <c r="J112" t="s">
+        <v>840</v>
+      </c>
+      <c r="K112">
+        <v>219</v>
+      </c>
+      <c r="L112" t="s">
+        <v>841</v>
+      </c>
+      <c r="M112">
+        <v>396</v>
+      </c>
+      <c r="N112" t="s">
+        <v>842</v>
+      </c>
+      <c r="O112">
+        <v>187</v>
+      </c>
+      <c r="P112" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="113" spans="5:17">
+      <c r="E113" t="s">
+        <v>838</v>
+      </c>
+      <c r="F113" t="s">
+        <v>750</v>
+      </c>
+      <c r="G113" t="s">
+        <v>834</v>
+      </c>
+      <c r="H113" t="s">
+        <v>839</v>
+      </c>
+      <c r="I113">
+        <v>254</v>
+      </c>
+      <c r="J113" t="s">
+        <v>840</v>
+      </c>
+      <c r="K113">
+        <v>906</v>
+      </c>
+      <c r="L113" t="s">
+        <v>841</v>
+      </c>
+      <c r="M113">
+        <v>230</v>
+      </c>
+      <c r="N113" t="s">
+        <v>842</v>
+      </c>
+      <c r="O113">
+        <v>875</v>
+      </c>
+      <c r="P113" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="114" spans="5:17">
+      <c r="E114" t="s">
+        <v>838</v>
+      </c>
+      <c r="F114" t="s">
+        <v>750</v>
+      </c>
+      <c r="G114" t="s">
+        <v>834</v>
+      </c>
+      <c r="H114" t="s">
+        <v>839</v>
+      </c>
+      <c r="I114">
+        <v>429</v>
+      </c>
+      <c r="J114" t="s">
+        <v>840</v>
+      </c>
+      <c r="K114">
+        <v>906</v>
+      </c>
+      <c r="L114" t="s">
+        <v>841</v>
+      </c>
+      <c r="M114">
+        <v>405</v>
+      </c>
+      <c r="N114" t="s">
+        <v>842</v>
+      </c>
+      <c r="O114">
+        <v>875</v>
+      </c>
+      <c r="P114" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="115" spans="5:17">
+      <c r="E115" t="s">
+        <v>838</v>
+      </c>
+      <c r="F115" t="s">
+        <v>750</v>
+      </c>
+      <c r="G115" t="s">
+        <v>834</v>
+      </c>
+      <c r="H115" t="s">
+        <v>839</v>
+      </c>
+      <c r="I115">
+        <v>580</v>
+      </c>
+      <c r="J115" t="s">
+        <v>840</v>
+      </c>
+      <c r="K115">
+        <v>906</v>
+      </c>
+      <c r="L115" t="s">
+        <v>841</v>
+      </c>
+      <c r="M115">
+        <v>556</v>
+      </c>
+      <c r="N115" t="s">
+        <v>842</v>
+      </c>
+      <c r="O115">
+        <v>875</v>
+      </c>
+      <c r="P115" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="116" spans="5:17">
+      <c r="E116" t="s">
+        <v>838</v>
+      </c>
+      <c r="F116" t="s">
+        <v>750</v>
+      </c>
+      <c r="G116" t="s">
+        <v>834</v>
+      </c>
+      <c r="H116" t="s">
+        <v>839</v>
+      </c>
+      <c r="I116">
+        <v>705</v>
+      </c>
+      <c r="J116" t="s">
+        <v>840</v>
+      </c>
+      <c r="K116">
+        <v>217</v>
+      </c>
+      <c r="L116" t="s">
+        <v>841</v>
+      </c>
+      <c r="M116">
+        <v>681</v>
+      </c>
+      <c r="N116" t="s">
+        <v>842</v>
+      </c>
+      <c r="O116">
+        <v>186</v>
+      </c>
+      <c r="P116" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="117" spans="5:17">
+      <c r="E117" t="s">
+        <v>838</v>
+      </c>
+      <c r="F117" t="s">
+        <v>750</v>
+      </c>
+      <c r="G117" t="s">
+        <v>834</v>
+      </c>
+      <c r="H117" t="s">
+        <v>839</v>
+      </c>
+      <c r="I117">
+        <v>222</v>
+      </c>
+      <c r="J117" t="s">
+        <v>840</v>
+      </c>
+      <c r="K117">
+        <v>222</v>
+      </c>
+      <c r="L117" t="s">
+        <v>841</v>
+      </c>
+      <c r="M117">
+        <v>249</v>
+      </c>
+      <c r="N117" t="s">
+        <v>842</v>
+      </c>
+      <c r="O117">
+        <v>190</v>
+      </c>
+      <c r="P117" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="118" spans="5:17">
+      <c r="E118" t="s">
+        <v>838</v>
+      </c>
+      <c r="F118" t="s">
+        <v>750</v>
+      </c>
+      <c r="G118" t="s">
+        <v>834</v>
+      </c>
+      <c r="H118" t="s">
+        <v>839</v>
+      </c>
+      <c r="I118">
+        <v>178</v>
+      </c>
+      <c r="J118" t="s">
+        <v>840</v>
+      </c>
+      <c r="K118">
+        <v>904</v>
+      </c>
+      <c r="L118" t="s">
+        <v>841</v>
+      </c>
+      <c r="M118">
+        <v>204</v>
+      </c>
+      <c r="N118" t="s">
+        <v>842</v>
+      </c>
+      <c r="O118">
+        <v>873</v>
+      </c>
+      <c r="P118" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="119" spans="5:17">
+      <c r="E119" t="s">
+        <v>838</v>
+      </c>
+      <c r="F119" t="s">
+        <v>750</v>
+      </c>
+      <c r="G119" t="s">
+        <v>834</v>
+      </c>
+      <c r="H119" t="s">
+        <v>839</v>
+      </c>
+      <c r="I119">
+        <v>357</v>
+      </c>
+      <c r="J119" t="s">
+        <v>840</v>
+      </c>
+      <c r="K119">
+        <v>909</v>
+      </c>
+      <c r="L119" t="s">
+        <v>841</v>
+      </c>
+      <c r="M119">
+        <v>384</v>
+      </c>
+      <c r="N119" t="s">
+        <v>842</v>
+      </c>
+      <c r="O119">
+        <v>878</v>
+      </c>
+      <c r="P119" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="120" spans="5:17">
+      <c r="E120" t="s">
+        <v>838</v>
+      </c>
+      <c r="F120" t="s">
+        <v>750</v>
+      </c>
+      <c r="G120" t="s">
+        <v>834</v>
+      </c>
+      <c r="H120" t="s">
+        <v>839</v>
+      </c>
+      <c r="I120">
+        <v>441</v>
+      </c>
+      <c r="J120" t="s">
+        <v>840</v>
+      </c>
+      <c r="K120">
+        <v>217</v>
+      </c>
+      <c r="L120" t="s">
+        <v>841</v>
+      </c>
+      <c r="M120">
+        <v>467</v>
+      </c>
+      <c r="N120" t="s">
+        <v>842</v>
+      </c>
+      <c r="O120">
+        <v>186</v>
+      </c>
+      <c r="P120" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="121" spans="5:17">
+      <c r="E121" t="s">
+        <v>838</v>
+      </c>
+      <c r="F121" t="s">
+        <v>750</v>
+      </c>
+      <c r="G121" t="s">
+        <v>834</v>
+      </c>
+      <c r="H121" t="s">
+        <v>839</v>
+      </c>
+      <c r="I121">
+        <v>732</v>
+      </c>
+      <c r="J121" t="s">
+        <v>840</v>
+      </c>
+      <c r="K121">
+        <v>219</v>
+      </c>
+      <c r="L121" t="s">
+        <v>841</v>
+      </c>
+      <c r="M121">
+        <v>759</v>
+      </c>
+      <c r="N121" t="s">
+        <v>842</v>
+      </c>
+      <c r="O121">
+        <v>187</v>
+      </c>
+      <c r="P121" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="122" spans="5:17">
+      <c r="E122" t="s">
+        <v>838</v>
+      </c>
+      <c r="F122" t="s">
+        <v>750</v>
+      </c>
+      <c r="G122" t="s">
+        <v>834</v>
+      </c>
+      <c r="H122" t="s">
+        <v>839</v>
+      </c>
+      <c r="I122">
+        <v>502</v>
+      </c>
+      <c r="J122" t="s">
+        <v>840</v>
+      </c>
+      <c r="K122">
+        <v>906</v>
+      </c>
+      <c r="L122" t="s">
+        <v>841</v>
+      </c>
+      <c r="M122">
+        <v>529</v>
+      </c>
+      <c r="N122" t="s">
+        <v>842</v>
+      </c>
+      <c r="O122">
+        <v>875</v>
+      </c>
+      <c r="P122" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="123" spans="5:17">
+      <c r="E123" t="s">
+        <v>838</v>
+      </c>
+      <c r="F123" t="s">
+        <v>750</v>
+      </c>
+      <c r="G123" t="s">
+        <v>834</v>
+      </c>
+      <c r="H123" t="s">
+        <v>839</v>
+      </c>
+      <c r="I123">
+        <v>370</v>
+      </c>
+      <c r="J123" t="s">
+        <v>840</v>
+      </c>
+      <c r="K123">
+        <v>1103</v>
+      </c>
+      <c r="L123" t="s">
+        <v>841</v>
+      </c>
+      <c r="M123">
+        <v>397</v>
+      </c>
+      <c r="N123" t="s">
+        <v>842</v>
+      </c>
+      <c r="O123">
+        <v>1072</v>
+      </c>
+      <c r="P123" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="124" spans="5:17">
+      <c r="E124" t="s">
+        <v>838</v>
+      </c>
+      <c r="F124" t="s">
+        <v>750</v>
+      </c>
+      <c r="G124" t="s">
+        <v>834</v>
+      </c>
+      <c r="H124" t="s">
+        <v>839</v>
+      </c>
+      <c r="I124">
+        <v>321</v>
+      </c>
+      <c r="J124" t="s">
+        <v>840</v>
+      </c>
+      <c r="K124">
+        <v>1432</v>
+      </c>
+      <c r="L124" t="s">
+        <v>841</v>
+      </c>
+      <c r="M124">
+        <v>348</v>
+      </c>
+      <c r="N124" t="s">
+        <v>842</v>
+      </c>
+      <c r="O124">
+        <v>1401</v>
+      </c>
+      <c r="P124" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="125" spans="5:17">
+      <c r="E125" t="s">
+        <v>838</v>
+      </c>
+      <c r="F125" t="s">
+        <v>750</v>
+      </c>
+      <c r="G125" t="s">
+        <v>834</v>
+      </c>
+      <c r="H125" t="s">
+        <v>839</v>
+      </c>
+      <c r="I125">
+        <v>551</v>
+      </c>
+      <c r="J125" t="s">
+        <v>840</v>
+      </c>
+      <c r="K125">
+        <v>1430</v>
+      </c>
+      <c r="L125" t="s">
+        <v>841</v>
+      </c>
+      <c r="M125">
+        <v>578</v>
+      </c>
+      <c r="N125" t="s">
+        <v>842</v>
+      </c>
+      <c r="O125">
+        <v>1399</v>
+      </c>
+      <c r="P125" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="126" spans="5:17">
+      <c r="E126" t="s">
+        <v>838</v>
+      </c>
+      <c r="F126" t="s">
+        <v>750</v>
+      </c>
+      <c r="G126" t="s">
+        <v>834</v>
+      </c>
+      <c r="H126" t="s">
+        <v>839</v>
+      </c>
+      <c r="I126">
+        <v>530</v>
+      </c>
+      <c r="J126" t="s">
+        <v>840</v>
+      </c>
+      <c r="K126">
+        <v>1103</v>
+      </c>
+      <c r="L126" t="s">
+        <v>841</v>
+      </c>
+      <c r="M126">
+        <v>506</v>
+      </c>
+      <c r="N126" t="s">
+        <v>842</v>
+      </c>
+      <c r="O126">
+        <v>1072</v>
+      </c>
+      <c r="P126" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="127" spans="5:17">
+      <c r="E127" t="s">
+        <v>838</v>
+      </c>
+      <c r="F127" t="s">
+        <v>750</v>
+      </c>
+      <c r="G127" t="s">
+        <v>834</v>
+      </c>
+      <c r="H127" t="s">
+        <v>839</v>
+      </c>
+      <c r="I127">
+        <v>644</v>
+      </c>
+      <c r="J127" t="s">
+        <v>840</v>
+      </c>
+      <c r="K127">
+        <v>1429</v>
+      </c>
+      <c r="L127" t="s">
+        <v>841</v>
+      </c>
+      <c r="M127">
+        <v>620</v>
+      </c>
+      <c r="N127" t="s">
+        <v>842</v>
+      </c>
+      <c r="O127">
+        <v>1398</v>
+      </c>
+      <c r="P127" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="128" spans="5:17">
+      <c r="E128" t="s">
+        <v>838</v>
+      </c>
+      <c r="F128" t="s">
+        <v>750</v>
+      </c>
+      <c r="G128" t="s">
+        <v>834</v>
+      </c>
+      <c r="H128" t="s">
+        <v>839</v>
+      </c>
+      <c r="I128">
+        <v>397</v>
+      </c>
+      <c r="J128" t="s">
+        <v>840</v>
+      </c>
+      <c r="K128">
+        <v>1427</v>
+      </c>
+      <c r="L128" t="s">
+        <v>841</v>
+      </c>
+      <c r="M128">
+        <v>373</v>
+      </c>
+      <c r="N128" t="s">
+        <v>842</v>
+      </c>
+      <c r="O128">
+        <v>1396</v>
+      </c>
+      <c r="P128" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="130" spans="5:28">
+      <c r="E130" t="s">
+        <v>833</v>
+      </c>
+      <c r="F130" t="s">
+        <v>750</v>
+      </c>
+      <c r="G130" t="s">
+        <v>834</v>
+      </c>
+      <c r="H130" t="s">
+        <v>835</v>
+      </c>
+      <c r="I130" t="s">
+        <v>861</v>
+      </c>
+      <c r="J130" t="s">
+        <v>2</v>
+      </c>
+      <c r="K130" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="133" spans="5:28">
+      <c r="E133" t="s">
+        <v>863</v>
+      </c>
+      <c r="F133" t="s">
+        <v>864</v>
+      </c>
+      <c r="G133" t="s">
+        <v>865</v>
+      </c>
+      <c r="H133" t="s">
+        <v>866</v>
+      </c>
+      <c r="I133" t="s">
+        <v>865</v>
+      </c>
+      <c r="J133" t="s">
+        <v>867</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133" t="s">
+        <v>174</v>
+      </c>
+      <c r="M133">
+        <v>369</v>
+      </c>
+      <c r="N133" t="s">
+        <v>175</v>
+      </c>
+      <c r="O133">
+        <v>868</v>
+      </c>
+      <c r="P133" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>868</v>
+      </c>
+      <c r="R133" t="s">
+        <v>869</v>
+      </c>
+      <c r="S133">
+        <v>24</v>
+      </c>
+      <c r="T133" t="s">
+        <v>870</v>
+      </c>
+      <c r="U133" t="s">
+        <v>871</v>
+      </c>
+      <c r="V133" t="s">
+        <v>872</v>
+      </c>
+      <c r="W133" t="s">
+        <v>873</v>
+      </c>
+      <c r="X133" t="s">
+        <v>874</v>
+      </c>
+      <c r="Y133" t="s">
+        <v>875</v>
+      </c>
+      <c r="Z133" t="s">
+        <v>757</v>
+      </c>
+      <c r="AA133" t="s">
+        <v>876</v>
+      </c>
+      <c r="AB133" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="135" spans="5:28">
+      <c r="E135" t="s">
+        <v>863</v>
+      </c>
+      <c r="F135" t="s">
+        <v>864</v>
+      </c>
+      <c r="G135" t="s">
+        <v>865</v>
+      </c>
+      <c r="H135" t="s">
+        <v>866</v>
+      </c>
+      <c r="I135" t="s">
+        <v>865</v>
+      </c>
+      <c r="J135" t="s">
+        <v>867</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135" t="s">
+        <v>174</v>
+      </c>
+      <c r="M135">
+        <v>360</v>
+      </c>
+      <c r="N135" t="s">
+        <v>175</v>
+      </c>
+      <c r="O135">
+        <v>1103</v>
+      </c>
+      <c r="P135" t="s">
+        <v>869</v>
+      </c>
+      <c r="Q135">
+        <v>24</v>
+      </c>
+      <c r="R135" t="s">
+        <v>870</v>
+      </c>
+      <c r="S135" t="s">
+        <v>871</v>
+      </c>
+      <c r="T135" t="s">
+        <v>872</v>
+      </c>
+      <c r="U135" t="s">
+        <v>873</v>
+      </c>
+      <c r="V135" t="s">
+        <v>874</v>
+      </c>
+      <c r="W135" t="s">
+        <v>875</v>
+      </c>
+      <c r="X135" t="s">
+        <v>757</v>
+      </c>
+      <c r="Y135" t="s">
+        <v>878</v>
+      </c>
+      <c r="Z135" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA135" t="s">
+        <v>879</v>
+      </c>
+      <c r="AB135" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="140" spans="5:28">
+      <c r="E140" t="s">
+        <v>838</v>
+      </c>
+      <c r="F140" t="s">
+        <v>750</v>
+      </c>
+      <c r="G140" t="s">
+        <v>834</v>
+      </c>
+      <c r="H140" t="s">
+        <v>2</v>
+      </c>
+      <c r="I140" t="s">
+        <v>880</v>
+      </c>
+      <c r="J140" t="s">
+        <v>842</v>
+      </c>
+      <c r="K140">
+        <v>-587</v>
+      </c>
+      <c r="L140" t="s">
+        <v>841</v>
+      </c>
+      <c r="M140">
+        <v>23</v>
+      </c>
+      <c r="N140" t="s">
+        <v>840</v>
+      </c>
+      <c r="O140">
+        <v>-587</v>
+      </c>
+      <c r="P140" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="141" spans="5:28">
+      <c r="E141" t="s">
+        <v>838</v>
+      </c>
+      <c r="F141" t="s">
+        <v>750</v>
+      </c>
+      <c r="G141" t="s">
+        <v>834</v>
+      </c>
+      <c r="H141" t="s">
+        <v>2</v>
+      </c>
+      <c r="I141" t="s">
+        <v>882</v>
+      </c>
+      <c r="J141" t="s">
+        <v>842</v>
+      </c>
+      <c r="K141">
+        <v>-242</v>
+      </c>
+      <c r="L141" t="s">
+        <v>841</v>
+      </c>
+      <c r="M141">
+        <v>19</v>
+      </c>
+      <c r="N141" t="s">
+        <v>840</v>
+      </c>
+      <c r="O141">
+        <v>-242</v>
+      </c>
+      <c r="P141" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="142" spans="5:28">
+      <c r="E142" t="s">
+        <v>838</v>
+      </c>
+      <c r="F142" t="s">
+        <v>750</v>
+      </c>
+      <c r="G142" t="s">
+        <v>834</v>
+      </c>
+      <c r="H142" t="s">
+        <v>2</v>
+      </c>
+      <c r="I142" t="s">
+        <v>884</v>
+      </c>
+      <c r="J142" t="s">
+        <v>842</v>
+      </c>
+      <c r="K142">
+        <v>89</v>
+      </c>
+      <c r="L142" t="s">
+        <v>841</v>
+      </c>
+      <c r="M142">
+        <v>18</v>
+      </c>
+      <c r="N142" t="s">
+        <v>840</v>
+      </c>
+      <c r="O142">
+        <v>89</v>
+      </c>
+      <c r="P142" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="143" spans="5:28">
+      <c r="E143" t="s">
+        <v>838</v>
+      </c>
+      <c r="F143" t="s">
+        <v>750</v>
+      </c>
+      <c r="G143" t="s">
+        <v>834</v>
+      </c>
+      <c r="H143" t="s">
+        <v>2</v>
+      </c>
+      <c r="I143" t="s">
+        <v>886</v>
+      </c>
+      <c r="J143" t="s">
+        <v>842</v>
+      </c>
+      <c r="K143">
+        <v>-319</v>
+      </c>
+      <c r="L143" t="s">
+        <v>841</v>
+      </c>
+      <c r="M143">
+        <v>425</v>
+      </c>
+      <c r="N143" t="s">
+        <v>840</v>
+      </c>
+      <c r="O143">
+        <v>-319</v>
+      </c>
+      <c r="P143" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="144" spans="5:28">
+      <c r="E144" t="s">
+        <v>838</v>
+      </c>
+      <c r="F144" t="s">
+        <v>750</v>
+      </c>
+      <c r="G144" t="s">
+        <v>834</v>
+      </c>
+      <c r="H144" t="s">
+        <v>2</v>
+      </c>
+      <c r="I144" t="s">
+        <v>888</v>
+      </c>
+      <c r="J144" t="s">
+        <v>842</v>
+      </c>
+      <c r="K144">
+        <v>-239</v>
+      </c>
+      <c r="L144" t="s">
+        <v>841</v>
+      </c>
+      <c r="M144">
+        <v>442</v>
+      </c>
+      <c r="N144" t="s">
+        <v>840</v>
+      </c>
+      <c r="O144">
+        <v>-239</v>
+      </c>
+      <c r="P144" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="145" spans="5:17">
+      <c r="E145" t="s">
+        <v>838</v>
+      </c>
+      <c r="F145" t="s">
+        <v>750</v>
+      </c>
+      <c r="G145" t="s">
+        <v>834</v>
+      </c>
+      <c r="H145" t="s">
+        <v>2</v>
+      </c>
+      <c r="I145" t="s">
+        <v>890</v>
+      </c>
+      <c r="J145" t="s">
+        <v>842</v>
+      </c>
+      <c r="K145">
+        <v>71</v>
+      </c>
+      <c r="L145" t="s">
+        <v>841</v>
+      </c>
+      <c r="M145">
+        <v>481</v>
+      </c>
+      <c r="N145" t="s">
+        <v>840</v>
+      </c>
+      <c r="O145">
+        <v>71</v>
+      </c>
+      <c r="P145" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="146" spans="5:17">
+      <c r="E146" t="s">
+        <v>838</v>
+      </c>
+      <c r="F146" t="s">
+        <v>750</v>
+      </c>
+      <c r="G146" t="s">
+        <v>834</v>
+      </c>
+      <c r="H146" t="s">
+        <v>2</v>
+      </c>
+      <c r="I146" t="s">
+        <v>892</v>
+      </c>
+      <c r="J146" t="s">
+        <v>842</v>
+      </c>
+      <c r="K146">
+        <v>-800</v>
+      </c>
+      <c r="L146" t="s">
+        <v>841</v>
+      </c>
+      <c r="M146">
+        <v>24</v>
+      </c>
+      <c r="N146" t="s">
+        <v>840</v>
+      </c>
+      <c r="O146">
+        <v>-800</v>
+      </c>
+      <c r="P146" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="147" spans="5:17">
+      <c r="E147" t="s">
+        <v>838</v>
+      </c>
+      <c r="F147" t="s">
+        <v>750</v>
+      </c>
+      <c r="G147" t="s">
+        <v>834</v>
+      </c>
+      <c r="H147" t="s">
+        <v>2</v>
+      </c>
+      <c r="I147" t="s">
+        <v>894</v>
+      </c>
+      <c r="J147" t="s">
+        <v>842</v>
+      </c>
+      <c r="K147">
+        <v>-319</v>
+      </c>
+      <c r="L147" t="s">
+        <v>841</v>
+      </c>
+      <c r="M147">
+        <v>428</v>
+      </c>
+      <c r="N147" t="s">
+        <v>840</v>
+      </c>
+      <c r="O147">
+        <v>-800</v>
+      </c>
+      <c r="P147" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="148" spans="5:17">
+      <c r="E148" t="s">
+        <v>838</v>
+      </c>
+      <c r="F148" t="s">
+        <v>750</v>
+      </c>
+      <c r="G148" t="s">
+        <v>834</v>
+      </c>
+      <c r="H148" t="s">
+        <v>2</v>
+      </c>
+      <c r="I148" t="s">
+        <v>896</v>
+      </c>
+      <c r="J148" t="s">
+        <v>842</v>
+      </c>
+      <c r="K148">
+        <v>87</v>
+      </c>
+      <c r="L148" t="s">
+        <v>841</v>
+      </c>
+      <c r="M148">
+        <v>22</v>
+      </c>
+      <c r="N148" t="s">
+        <v>840</v>
+      </c>
+      <c r="O148">
+        <v>-799</v>
+      </c>
+      <c r="P148" t="s">
+        <v>839</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="149" spans="5:17">
+      <c r="E149" t="s">
+        <v>838</v>
+      </c>
+      <c r="F149" t="s">
+        <v>750</v>
+      </c>
+      <c r="G149" t="s">
+        <v>834</v>
+      </c>
+      <c r="H149" t="s">
+        <v>839</v>
+      </c>
+      <c r="I149">
+        <v>652</v>
+      </c>
+      <c r="J149" t="s">
+        <v>840</v>
+      </c>
+      <c r="K149">
+        <v>-240</v>
+      </c>
+      <c r="L149" t="s">
+        <v>841</v>
+      </c>
+      <c r="M149">
+        <v>652</v>
+      </c>
+      <c r="N149" t="s">
+        <v>842</v>
+      </c>
+      <c r="O149">
+        <v>71</v>
+      </c>
+      <c r="P149" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="152" spans="5:17">
+      <c r="E152" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="153" spans="5:17">
+      <c r="E153" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="155" spans="5:17">
+      <c r="E155" t="s">
+        <v>900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated company grid data js to match xls sheet
</commit_message>
<xml_diff>
--- a/full-data-iday14.xlsx
+++ b/full-data-iday14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="-440" windowWidth="14360" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="11100" yWindow="40" windowWidth="14360" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="905">
   <si>
     <t>booth</t>
   </si>
@@ -5058,8 +5058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5901,8 +5901,8 @@
       <c r="A12" s="150">
         <v>19</v>
       </c>
-      <c r="B12" s="180" t="s">
-        <v>705</v>
+      <c r="B12" s="198">
+        <v>233024</v>
       </c>
       <c r="C12" s="160">
         <v>1160</v>

</xml_diff>

<commit_message>
blreg kinda redoing booths
</commit_message>
<xml_diff>
--- a/full-data-iday14.xlsx
+++ b/full-data-iday14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="40" windowWidth="14360" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="alt company names" sheetId="2" r:id="rId5"/>
     <sheet name="booth layout prev" sheetId="3" r:id="rId6"/>
     <sheet name="nonfinaldata" sheetId="4" r:id="rId7"/>
+    <sheet name="more booth udpates" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">current!$F$1:$T$74</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="976">
   <si>
     <t>booth</t>
   </si>
@@ -2743,13 +2744,226 @@
   </si>
   <si>
     <t>chrysler</t>
+  </si>
+  <si>
+    <t>&lt;svg</t>
+  </si>
+  <si>
+    <t>viewBox</t>
+  </si>
+  <si>
+    <t>-10 -800 1000 2225</t>
+  </si>
+  <si>
+    <t>xmlns</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/svg</t>
+  </si>
+  <si>
+    <t>xmlns:svg</t>
+  </si>
+  <si>
+    <t>xmlns:xlink</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/xlink&gt;</t>
+  </si>
+  <si>
+    <t>&lt;image</t>
+  </si>
+  <si>
+    <t>xlink:href</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/ArXl22P.png</t>
+  </si>
+  <si>
+    <t>svg_1</t>
+  </si>
+  <si>
+    <t>8/&gt;</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/HphIdr8.png</t>
+  </si>
+  <si>
+    <t>svg_2</t>
+  </si>
+  <si>
+    <t>5/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;g</t>
+  </si>
+  <si>
+    <t>svg_19&gt;</t>
+  </si>
+  <si>
+    <t>booth6</t>
+  </si>
+  <si>
+    <t>booth7</t>
+  </si>
+  <si>
+    <t>booth4</t>
+  </si>
+  <si>
+    <t>booth9</t>
+  </si>
+  <si>
+    <t>booth10</t>
+  </si>
+  <si>
+    <t>booth3</t>
+  </si>
+  <si>
+    <t>booth5</t>
+  </si>
+  <si>
+    <t>booth8</t>
+  </si>
+  <si>
+    <t>booth42/&gt;</t>
+  </si>
+  <si>
+    <t>booth43/&gt;</t>
+  </si>
+  <si>
+    <t>booth44/&gt;</t>
+  </si>
+  <si>
+    <t>booth45/&gt;</t>
+  </si>
+  <si>
+    <t>booth46/&gt;</t>
+  </si>
+  <si>
+    <t>booth49/&gt;</t>
+  </si>
+  <si>
+    <t>booth50/&gt;</t>
+  </si>
+  <si>
+    <t>booth48/&gt;</t>
+  </si>
+  <si>
+    <t>booth51/&gt;</t>
+  </si>
+  <si>
+    <t>booth47/&gt;</t>
+  </si>
+  <si>
+    <t>booth52/&gt;</t>
+  </si>
+  <si>
+    <t>booth40/&gt;</t>
+  </si>
+  <si>
+    <t>booth39/&gt;</t>
+  </si>
+  <si>
+    <t>booth38/&gt;</t>
+  </si>
+  <si>
+    <t>booth59/&gt;</t>
+  </si>
+  <si>
+    <t>booth60/&gt;</t>
+  </si>
+  <si>
+    <t>booth58/&gt;</t>
+  </si>
+  <si>
+    <t>booth61/&gt;</t>
+  </si>
+  <si>
+    <t>booth57/&gt;</t>
+  </si>
+  <si>
+    <t>booth62/&gt;</t>
+  </si>
+  <si>
+    <t>booth36/&gt;</t>
+  </si>
+  <si>
+    <t>booth35/&gt;</t>
+  </si>
+  <si>
+    <t>booth34/&gt;</t>
+  </si>
+  <si>
+    <t>booth33/&gt;</t>
+  </si>
+  <si>
+    <t>booth32/&gt;</t>
+  </si>
+  <si>
+    <t>booth54/&gt;</t>
+  </si>
+  <si>
+    <t>booth55/&gt;</t>
+  </si>
+  <si>
+    <t>booth53/&gt;</t>
+  </si>
+  <si>
+    <t>booth56/&gt;</t>
+  </si>
+  <si>
+    <t>booth10/&gt;</t>
+  </si>
+  <si>
+    <t>booth11/&gt;</t>
+  </si>
+  <si>
+    <t>booth15/&gt;</t>
+  </si>
+  <si>
+    <t>booth12/&gt;</t>
+  </si>
+  <si>
+    <t>booth13/&gt;</t>
+  </si>
+  <si>
+    <t>booth14/&gt;</t>
+  </si>
+  <si>
+    <t>booth16/&gt;</t>
+  </si>
+  <si>
+    <t>booth25</t>
+  </si>
+  <si>
+    <t>booth26</t>
+  </si>
+  <si>
+    <t>booth22</t>
+  </si>
+  <si>
+    <t>booth2027/&gt;</t>
+  </si>
+  <si>
+    <t>booth2720</t>
+  </si>
+  <si>
+    <t>booth24</t>
+  </si>
+  <si>
+    <t>&lt;/g&gt;</t>
+  </si>
+  <si>
+    <t>20-27</t>
+  </si>
+  <si>
+    <t>27-20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2924,6 +3138,13 @@
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3600,7 +3821,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="295">
+  <cellStyleXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3896,8 +4117,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4431,8 +4654,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="295">
+  <cellStyles count="297">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4579,6 +4803,7 @@
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -4725,6 +4950,7 @@
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Output" xfId="70" builtinId="21"/>
@@ -5058,7 +5284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -23746,4 +23972,2423 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X163"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89:J95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C1">
+        <v>1100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>748</v>
+      </c>
+      <c r="E1">
+        <v>2435</v>
+      </c>
+      <c r="F1" t="s">
+        <v>906</v>
+      </c>
+      <c r="G1" t="s">
+        <v>907</v>
+      </c>
+      <c r="H1" t="s">
+        <v>908</v>
+      </c>
+      <c r="I1" t="s">
+        <v>909</v>
+      </c>
+      <c r="J1" t="s">
+        <v>910</v>
+      </c>
+      <c r="K1" t="s">
+        <v>909</v>
+      </c>
+      <c r="L1" t="s">
+        <v>911</v>
+      </c>
+      <c r="M1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>913</v>
+      </c>
+      <c r="B2" t="s">
+        <v>914</v>
+      </c>
+      <c r="C2" t="s">
+        <v>915</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>916</v>
+      </c>
+      <c r="F2" t="s">
+        <v>748</v>
+      </c>
+      <c r="G2">
+        <v>1248</v>
+      </c>
+      <c r="H2" t="s">
+        <v>749</v>
+      </c>
+      <c r="I2">
+        <v>953</v>
+      </c>
+      <c r="J2" t="s">
+        <v>175</v>
+      </c>
+      <c r="K2">
+        <v>185</v>
+      </c>
+      <c r="L2" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>913</v>
+      </c>
+      <c r="B3" t="s">
+        <v>914</v>
+      </c>
+      <c r="C3" t="s">
+        <v>918</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>919</v>
+      </c>
+      <c r="F3" t="s">
+        <v>748</v>
+      </c>
+      <c r="G3">
+        <v>2251</v>
+      </c>
+      <c r="H3" t="s">
+        <v>749</v>
+      </c>
+      <c r="I3">
+        <v>964</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3">
+        <v>-818</v>
+      </c>
+      <c r="L3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>833</v>
+      </c>
+      <c r="B6" t="s">
+        <v>750</v>
+      </c>
+      <c r="C6" t="s">
+        <v>834</v>
+      </c>
+      <c r="D6" t="s">
+        <v>835</v>
+      </c>
+      <c r="E6" t="s">
+        <v>836</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" t="s">
+        <v>833</v>
+      </c>
+      <c r="B7" t="s">
+        <v>750</v>
+      </c>
+      <c r="C7" t="s">
+        <v>834</v>
+      </c>
+      <c r="D7" t="s">
+        <v>835</v>
+      </c>
+      <c r="E7" t="s">
+        <v>861</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>863</v>
+      </c>
+      <c r="B9" t="s">
+        <v>864</v>
+      </c>
+      <c r="C9" t="s">
+        <v>865</v>
+      </c>
+      <c r="D9" t="s">
+        <v>866</v>
+      </c>
+      <c r="E9" t="s">
+        <v>865</v>
+      </c>
+      <c r="F9" t="s">
+        <v>867</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9">
+        <v>369</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9">
+        <v>868</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>868</v>
+      </c>
+      <c r="N9" t="s">
+        <v>869</v>
+      </c>
+      <c r="O9">
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>870</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>871</v>
+      </c>
+      <c r="R9" t="s">
+        <v>872</v>
+      </c>
+      <c r="S9" t="s">
+        <v>873</v>
+      </c>
+      <c r="T9" t="s">
+        <v>874</v>
+      </c>
+      <c r="U9" t="s">
+        <v>875</v>
+      </c>
+      <c r="V9" t="s">
+        <v>757</v>
+      </c>
+      <c r="W9" t="s">
+        <v>876</v>
+      </c>
+      <c r="X9" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" t="s">
+        <v>863</v>
+      </c>
+      <c r="B11" t="s">
+        <v>864</v>
+      </c>
+      <c r="C11" t="s">
+        <v>865</v>
+      </c>
+      <c r="D11" t="s">
+        <v>866</v>
+      </c>
+      <c r="E11" t="s">
+        <v>865</v>
+      </c>
+      <c r="F11" t="s">
+        <v>867</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>174</v>
+      </c>
+      <c r="I11">
+        <v>360</v>
+      </c>
+      <c r="J11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11">
+        <v>1103</v>
+      </c>
+      <c r="L11" t="s">
+        <v>869</v>
+      </c>
+      <c r="M11">
+        <v>24</v>
+      </c>
+      <c r="N11" t="s">
+        <v>870</v>
+      </c>
+      <c r="O11" t="s">
+        <v>871</v>
+      </c>
+      <c r="P11" t="s">
+        <v>872</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>873</v>
+      </c>
+      <c r="R11" t="s">
+        <v>874</v>
+      </c>
+      <c r="S11" t="s">
+        <v>875</v>
+      </c>
+      <c r="T11" t="s">
+        <v>757</v>
+      </c>
+      <c r="U11" t="s">
+        <v>878</v>
+      </c>
+      <c r="V11" t="s">
+        <v>2</v>
+      </c>
+      <c r="W11" t="s">
+        <v>879</v>
+      </c>
+      <c r="X11" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="E12" t="s">
+        <v>839</v>
+      </c>
+      <c r="G12" t="s">
+        <v>840</v>
+      </c>
+      <c r="I12" t="s">
+        <v>841</v>
+      </c>
+      <c r="K12" t="s">
+        <v>842</v>
+      </c>
+      <c r="M12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" t="s">
+        <v>838</v>
+      </c>
+      <c r="B13" t="s">
+        <v>750</v>
+      </c>
+      <c r="C13" t="s">
+        <v>834</v>
+      </c>
+      <c r="E13">
+        <v>202</v>
+      </c>
+      <c r="G13">
+        <v>218</v>
+      </c>
+      <c r="I13">
+        <v>178</v>
+      </c>
+      <c r="K13">
+        <v>186</v>
+      </c>
+      <c r="M13" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="E14">
+        <v>420</v>
+      </c>
+      <c r="G14">
+        <v>219</v>
+      </c>
+      <c r="I14">
+        <v>396</v>
+      </c>
+      <c r="K14">
+        <v>187</v>
+      </c>
+      <c r="M14" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="E15">
+        <v>254</v>
+      </c>
+      <c r="G15">
+        <v>906</v>
+      </c>
+      <c r="I15">
+        <v>230</v>
+      </c>
+      <c r="K15">
+        <v>875</v>
+      </c>
+      <c r="M15" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="E16">
+        <v>429</v>
+      </c>
+      <c r="G16">
+        <v>906</v>
+      </c>
+      <c r="I16">
+        <v>405</v>
+      </c>
+      <c r="K16">
+        <v>875</v>
+      </c>
+      <c r="M16" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14">
+      <c r="E17">
+        <v>580</v>
+      </c>
+      <c r="G17">
+        <v>906</v>
+      </c>
+      <c r="I17">
+        <v>556</v>
+      </c>
+      <c r="K17">
+        <v>875</v>
+      </c>
+      <c r="M17" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14">
+      <c r="E18">
+        <v>705</v>
+      </c>
+      <c r="G18">
+        <v>217</v>
+      </c>
+      <c r="I18">
+        <v>681</v>
+      </c>
+      <c r="K18">
+        <v>186</v>
+      </c>
+      <c r="M18" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14">
+      <c r="E19">
+        <v>222</v>
+      </c>
+      <c r="G19">
+        <v>222</v>
+      </c>
+      <c r="I19">
+        <v>249</v>
+      </c>
+      <c r="K19">
+        <v>190</v>
+      </c>
+      <c r="M19" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14">
+      <c r="E20">
+        <v>178</v>
+      </c>
+      <c r="G20">
+        <v>904</v>
+      </c>
+      <c r="I20">
+        <v>204</v>
+      </c>
+      <c r="K20">
+        <v>873</v>
+      </c>
+      <c r="M20" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="21" spans="5:14">
+      <c r="E21">
+        <v>357</v>
+      </c>
+      <c r="G21">
+        <v>909</v>
+      </c>
+      <c r="I21">
+        <v>384</v>
+      </c>
+      <c r="K21">
+        <v>878</v>
+      </c>
+      <c r="M21" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14">
+      <c r="E22">
+        <v>441</v>
+      </c>
+      <c r="G22">
+        <v>217</v>
+      </c>
+      <c r="I22">
+        <v>467</v>
+      </c>
+      <c r="K22">
+        <v>186</v>
+      </c>
+      <c r="M22" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14">
+      <c r="E23">
+        <v>732</v>
+      </c>
+      <c r="G23">
+        <v>219</v>
+      </c>
+      <c r="I23">
+        <v>759</v>
+      </c>
+      <c r="K23">
+        <v>187</v>
+      </c>
+      <c r="M23" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14">
+      <c r="E24">
+        <v>502</v>
+      </c>
+      <c r="G24">
+        <v>906</v>
+      </c>
+      <c r="I24">
+        <v>529</v>
+      </c>
+      <c r="K24">
+        <v>875</v>
+      </c>
+      <c r="M24" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14">
+      <c r="E25">
+        <v>370</v>
+      </c>
+      <c r="G25">
+        <v>1103</v>
+      </c>
+      <c r="I25">
+        <v>397</v>
+      </c>
+      <c r="K25">
+        <v>1072</v>
+      </c>
+      <c r="M25" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="26" spans="5:14">
+      <c r="E26">
+        <v>321</v>
+      </c>
+      <c r="G26">
+        <v>1432</v>
+      </c>
+      <c r="I26">
+        <v>348</v>
+      </c>
+      <c r="K26">
+        <v>1401</v>
+      </c>
+      <c r="M26" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14">
+      <c r="E27">
+        <v>551</v>
+      </c>
+      <c r="G27">
+        <v>1430</v>
+      </c>
+      <c r="I27">
+        <v>578</v>
+      </c>
+      <c r="K27">
+        <v>1399</v>
+      </c>
+      <c r="M27" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14">
+      <c r="E28">
+        <v>530</v>
+      </c>
+      <c r="G28">
+        <v>1103</v>
+      </c>
+      <c r="I28">
+        <v>506</v>
+      </c>
+      <c r="K28">
+        <v>1072</v>
+      </c>
+      <c r="M28" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14">
+      <c r="E29">
+        <v>644</v>
+      </c>
+      <c r="G29">
+        <v>1429</v>
+      </c>
+      <c r="I29">
+        <v>620</v>
+      </c>
+      <c r="K29">
+        <v>1398</v>
+      </c>
+      <c r="M29" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="30" spans="5:14">
+      <c r="E30">
+        <v>397</v>
+      </c>
+      <c r="G30">
+        <v>1427</v>
+      </c>
+      <c r="I30">
+        <v>373</v>
+      </c>
+      <c r="K30">
+        <v>1396</v>
+      </c>
+      <c r="M30" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" ht="15">
+      <c r="E31" t="s">
+        <v>881</v>
+      </c>
+      <c r="G31">
+        <v>-587</v>
+      </c>
+      <c r="I31">
+        <v>23</v>
+      </c>
+      <c r="K31" s="201">
+        <v>-587</v>
+      </c>
+      <c r="M31" t="s">
+        <v>880</v>
+      </c>
+      <c r="N31" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="32" spans="5:14" ht="15">
+      <c r="E32" t="s">
+        <v>883</v>
+      </c>
+      <c r="G32">
+        <v>-242</v>
+      </c>
+      <c r="I32">
+        <v>19</v>
+      </c>
+      <c r="K32" s="201">
+        <v>-242</v>
+      </c>
+      <c r="M32" t="s">
+        <v>882</v>
+      </c>
+      <c r="N32" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15">
+      <c r="E33" t="s">
+        <v>885</v>
+      </c>
+      <c r="G33">
+        <v>89</v>
+      </c>
+      <c r="I33">
+        <v>18</v>
+      </c>
+      <c r="K33" s="201">
+        <v>89</v>
+      </c>
+      <c r="M33" t="s">
+        <v>884</v>
+      </c>
+      <c r="N33" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15">
+      <c r="E34" t="s">
+        <v>887</v>
+      </c>
+      <c r="G34">
+        <v>-319</v>
+      </c>
+      <c r="I34">
+        <v>425</v>
+      </c>
+      <c r="K34" s="201">
+        <v>-319</v>
+      </c>
+      <c r="M34" t="s">
+        <v>886</v>
+      </c>
+      <c r="N34" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15">
+      <c r="E35" t="s">
+        <v>889</v>
+      </c>
+      <c r="G35">
+        <v>-239</v>
+      </c>
+      <c r="I35">
+        <v>442</v>
+      </c>
+      <c r="K35" s="201">
+        <v>-239</v>
+      </c>
+      <c r="M35" t="s">
+        <v>888</v>
+      </c>
+      <c r="N35" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15">
+      <c r="E36" t="s">
+        <v>891</v>
+      </c>
+      <c r="G36">
+        <v>71</v>
+      </c>
+      <c r="I36">
+        <v>481</v>
+      </c>
+      <c r="K36" s="201">
+        <v>71</v>
+      </c>
+      <c r="M36" t="s">
+        <v>890</v>
+      </c>
+      <c r="N36" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15">
+      <c r="E37" t="s">
+        <v>893</v>
+      </c>
+      <c r="G37">
+        <v>-800</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="K37" s="201">
+        <v>-800</v>
+      </c>
+      <c r="M37" t="s">
+        <v>892</v>
+      </c>
+      <c r="N37" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15">
+      <c r="E38" t="s">
+        <v>895</v>
+      </c>
+      <c r="G38">
+        <v>-800</v>
+      </c>
+      <c r="I38">
+        <v>428</v>
+      </c>
+      <c r="K38" s="201">
+        <v>-319</v>
+      </c>
+      <c r="M38" t="s">
+        <v>894</v>
+      </c>
+      <c r="N38" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15">
+      <c r="E39" t="s">
+        <v>897</v>
+      </c>
+      <c r="G39">
+        <v>-799</v>
+      </c>
+      <c r="I39">
+        <v>22</v>
+      </c>
+      <c r="K39" s="201">
+        <v>87</v>
+      </c>
+      <c r="M39" t="s">
+        <v>896</v>
+      </c>
+      <c r="N39" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="E40">
+        <v>652</v>
+      </c>
+      <c r="G40">
+        <v>-240</v>
+      </c>
+      <c r="I40">
+        <v>652</v>
+      </c>
+      <c r="K40">
+        <v>71</v>
+      </c>
+      <c r="M40" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="B43" t="s">
+        <v>921</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
+        <v>746</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>923</v>
+      </c>
+      <c r="D44" t="s">
+        <v>748</v>
+      </c>
+      <c r="E44">
+        <v>21</v>
+      </c>
+      <c r="F44" t="s">
+        <v>749</v>
+      </c>
+      <c r="G44">
+        <v>56</v>
+      </c>
+      <c r="H44" t="s">
+        <v>175</v>
+      </c>
+      <c r="I44">
+        <v>-771</v>
+      </c>
+      <c r="J44" t="s">
+        <v>174</v>
+      </c>
+      <c r="K44">
+        <v>63</v>
+      </c>
+      <c r="L44" t="s">
+        <v>750</v>
+      </c>
+      <c r="M44" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>746</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>924</v>
+      </c>
+      <c r="D45" t="s">
+        <v>748</v>
+      </c>
+      <c r="E45">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>749</v>
+      </c>
+      <c r="G45">
+        <v>56</v>
+      </c>
+      <c r="H45" t="s">
+        <v>175</v>
+      </c>
+      <c r="I45">
+        <v>-766</v>
+      </c>
+      <c r="J45" t="s">
+        <v>174</v>
+      </c>
+      <c r="K45">
+        <v>293</v>
+      </c>
+      <c r="L45" t="s">
+        <v>750</v>
+      </c>
+      <c r="M45" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>746</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>925</v>
+      </c>
+      <c r="D46" t="s">
+        <v>748</v>
+      </c>
+      <c r="E46">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
+        <v>749</v>
+      </c>
+      <c r="G46">
+        <v>56</v>
+      </c>
+      <c r="H46" t="s">
+        <v>175</v>
+      </c>
+      <c r="I46">
+        <v>-534</v>
+      </c>
+      <c r="J46" t="s">
+        <v>174</v>
+      </c>
+      <c r="K46">
+        <v>59</v>
+      </c>
+      <c r="L46" t="s">
+        <v>750</v>
+      </c>
+      <c r="M46" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>746</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>926</v>
+      </c>
+      <c r="D47" t="s">
+        <v>748</v>
+      </c>
+      <c r="E47">
+        <v>21</v>
+      </c>
+      <c r="F47" t="s">
+        <v>749</v>
+      </c>
+      <c r="G47">
+        <v>56</v>
+      </c>
+      <c r="H47" t="s">
+        <v>175</v>
+      </c>
+      <c r="I47">
+        <v>96</v>
+      </c>
+      <c r="J47" t="s">
+        <v>174</v>
+      </c>
+      <c r="K47">
+        <v>539</v>
+      </c>
+      <c r="L47" t="s">
+        <v>750</v>
+      </c>
+      <c r="M47" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>746</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>927</v>
+      </c>
+      <c r="D48" t="s">
+        <v>748</v>
+      </c>
+      <c r="E48">
+        <v>21</v>
+      </c>
+      <c r="F48" t="s">
+        <v>749</v>
+      </c>
+      <c r="G48">
+        <v>56</v>
+      </c>
+      <c r="H48" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48">
+        <v>77</v>
+      </c>
+      <c r="J48" t="s">
+        <v>174</v>
+      </c>
+      <c r="K48">
+        <v>669</v>
+      </c>
+      <c r="L48" t="s">
+        <v>750</v>
+      </c>
+      <c r="M48" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" t="s">
+        <v>746</v>
+      </c>
+      <c r="B49" t="s">
+        <v>757</v>
+      </c>
+      <c r="C49" t="s">
+        <v>758</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>928</v>
+      </c>
+      <c r="F49" t="s">
+        <v>748</v>
+      </c>
+      <c r="G49">
+        <v>21</v>
+      </c>
+      <c r="H49" t="s">
+        <v>749</v>
+      </c>
+      <c r="I49">
+        <v>56</v>
+      </c>
+      <c r="J49" t="s">
+        <v>175</v>
+      </c>
+      <c r="K49">
+        <v>-387</v>
+      </c>
+      <c r="L49" t="s">
+        <v>174</v>
+      </c>
+      <c r="M49">
+        <v>32</v>
+      </c>
+      <c r="N49" t="s">
+        <v>750</v>
+      </c>
+      <c r="O49" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" t="s">
+        <v>746</v>
+      </c>
+      <c r="B50" t="s">
+        <v>750</v>
+      </c>
+      <c r="C50" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>929</v>
+      </c>
+      <c r="F50" t="s">
+        <v>757</v>
+      </c>
+      <c r="G50" t="s">
+        <v>761</v>
+      </c>
+      <c r="H50" t="s">
+        <v>748</v>
+      </c>
+      <c r="I50">
+        <v>21</v>
+      </c>
+      <c r="J50" t="s">
+        <v>749</v>
+      </c>
+      <c r="K50">
+        <v>56</v>
+      </c>
+      <c r="L50" t="s">
+        <v>175</v>
+      </c>
+      <c r="M50">
+        <v>-662</v>
+      </c>
+      <c r="N50" t="s">
+        <v>174</v>
+      </c>
+      <c r="O50" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" t="s">
+        <v>746</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>930</v>
+      </c>
+      <c r="D51" t="s">
+        <v>750</v>
+      </c>
+      <c r="E51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>757</v>
+      </c>
+      <c r="G51" t="s">
+        <v>764</v>
+      </c>
+      <c r="H51" t="s">
+        <v>748</v>
+      </c>
+      <c r="I51">
+        <v>21</v>
+      </c>
+      <c r="J51" t="s">
+        <v>749</v>
+      </c>
+      <c r="K51">
+        <v>56</v>
+      </c>
+      <c r="L51" t="s">
+        <v>175</v>
+      </c>
+      <c r="M51">
+        <v>-115</v>
+      </c>
+      <c r="N51" t="s">
+        <v>174</v>
+      </c>
+      <c r="O51" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52" t="s">
+        <v>746</v>
+      </c>
+      <c r="B52" t="s">
+        <v>757</v>
+      </c>
+      <c r="C52" t="s">
+        <v>766</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>765</v>
+      </c>
+      <c r="F52" t="s">
+        <v>748</v>
+      </c>
+      <c r="G52">
+        <v>21</v>
+      </c>
+      <c r="H52" t="s">
+        <v>749</v>
+      </c>
+      <c r="I52">
+        <v>56</v>
+      </c>
+      <c r="J52" t="s">
+        <v>175</v>
+      </c>
+      <c r="K52">
+        <v>-206</v>
+      </c>
+      <c r="L52" t="s">
+        <v>174</v>
+      </c>
+      <c r="M52">
+        <v>45</v>
+      </c>
+      <c r="N52" t="s">
+        <v>750</v>
+      </c>
+      <c r="O52" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" t="s">
+        <v>746</v>
+      </c>
+      <c r="B53" t="s">
+        <v>750</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>757</v>
+      </c>
+      <c r="E53" t="s">
+        <v>769</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" t="s">
+        <v>767</v>
+      </c>
+      <c r="H53" t="s">
+        <v>748</v>
+      </c>
+      <c r="I53">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>749</v>
+      </c>
+      <c r="K53">
+        <v>56</v>
+      </c>
+      <c r="L53" t="s">
+        <v>175</v>
+      </c>
+      <c r="M53">
+        <v>2</v>
+      </c>
+      <c r="N53" t="s">
+        <v>174</v>
+      </c>
+      <c r="O53" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" t="s">
+        <v>746</v>
+      </c>
+      <c r="B58" t="s">
+        <v>750</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>174</v>
+      </c>
+      <c r="F58" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" t="s">
+        <v>757</v>
+      </c>
+      <c r="J58" t="s">
+        <v>749</v>
+      </c>
+      <c r="K58" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="C59">
+        <v>42</v>
+      </c>
+      <c r="D59" t="s">
+        <v>931</v>
+      </c>
+      <c r="E59">
+        <v>41</v>
+      </c>
+      <c r="F59">
+        <v>332</v>
+      </c>
+      <c r="J59">
+        <v>21</v>
+      </c>
+      <c r="K59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="C60">
+        <v>43</v>
+      </c>
+      <c r="D60" t="s">
+        <v>932</v>
+      </c>
+      <c r="E60">
+        <v>40</v>
+      </c>
+      <c r="F60">
+        <v>425</v>
+      </c>
+      <c r="J60">
+        <v>21</v>
+      </c>
+      <c r="K60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="C61">
+        <v>44</v>
+      </c>
+      <c r="D61" t="s">
+        <v>933</v>
+      </c>
+      <c r="E61">
+        <v>43</v>
+      </c>
+      <c r="F61">
+        <v>513</v>
+      </c>
+      <c r="J61">
+        <v>18</v>
+      </c>
+      <c r="K61">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="C62">
+        <v>45</v>
+      </c>
+      <c r="D62" t="s">
+        <v>934</v>
+      </c>
+      <c r="E62">
+        <v>43</v>
+      </c>
+      <c r="F62">
+        <v>585</v>
+      </c>
+      <c r="J62">
+        <v>18</v>
+      </c>
+      <c r="K62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="C63">
+        <v>46</v>
+      </c>
+      <c r="D63" t="s">
+        <v>935</v>
+      </c>
+      <c r="E63">
+        <v>39</v>
+      </c>
+      <c r="F63">
+        <v>691</v>
+      </c>
+      <c r="J63">
+        <v>20</v>
+      </c>
+      <c r="K63">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="C64">
+        <v>49</v>
+      </c>
+      <c r="D64" t="s">
+        <v>936</v>
+      </c>
+      <c r="E64">
+        <v>238</v>
+      </c>
+      <c r="F64">
+        <v>382</v>
+      </c>
+      <c r="J64">
+        <v>22</v>
+      </c>
+      <c r="K64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11">
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="D65" t="s">
+        <v>937</v>
+      </c>
+      <c r="E65">
+        <v>281</v>
+      </c>
+      <c r="F65">
+        <v>378</v>
+      </c>
+      <c r="J65">
+        <v>27</v>
+      </c>
+      <c r="K65">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11">
+      <c r="C66">
+        <v>48</v>
+      </c>
+      <c r="D66" t="s">
+        <v>938</v>
+      </c>
+      <c r="E66">
+        <v>237</v>
+      </c>
+      <c r="F66">
+        <v>456</v>
+      </c>
+      <c r="J66">
+        <v>21</v>
+      </c>
+      <c r="K66">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="3:11">
+      <c r="C67">
+        <v>51</v>
+      </c>
+      <c r="D67" t="s">
+        <v>939</v>
+      </c>
+      <c r="E67">
+        <v>284</v>
+      </c>
+      <c r="F67">
+        <v>458</v>
+      </c>
+      <c r="J67">
+        <v>24</v>
+      </c>
+      <c r="K67">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11">
+      <c r="C68">
+        <v>47</v>
+      </c>
+      <c r="D68" t="s">
+        <v>940</v>
+      </c>
+      <c r="E68">
+        <v>235</v>
+      </c>
+      <c r="F68">
+        <v>541</v>
+      </c>
+      <c r="J68">
+        <v>22</v>
+      </c>
+      <c r="K68">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="3:11">
+      <c r="C69">
+        <v>52</v>
+      </c>
+      <c r="D69" t="s">
+        <v>941</v>
+      </c>
+      <c r="E69">
+        <v>283</v>
+      </c>
+      <c r="F69">
+        <v>542</v>
+      </c>
+      <c r="J69">
+        <v>27</v>
+      </c>
+      <c r="K69">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11">
+      <c r="C70">
+        <v>40</v>
+      </c>
+      <c r="D70" t="s">
+        <v>942</v>
+      </c>
+      <c r="E70">
+        <v>284</v>
+      </c>
+      <c r="F70">
+        <v>217</v>
+      </c>
+      <c r="J70">
+        <v>65</v>
+      </c>
+      <c r="K70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11">
+      <c r="C71">
+        <v>39</v>
+      </c>
+      <c r="D71" t="s">
+        <v>943</v>
+      </c>
+      <c r="E71">
+        <v>463</v>
+      </c>
+      <c r="F71">
+        <v>214</v>
+      </c>
+      <c r="J71">
+        <v>54</v>
+      </c>
+      <c r="K71">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11">
+      <c r="C72">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>944</v>
+      </c>
+      <c r="E72">
+        <v>576</v>
+      </c>
+      <c r="F72">
+        <v>216</v>
+      </c>
+      <c r="J72">
+        <v>56</v>
+      </c>
+      <c r="K72">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11">
+      <c r="C73">
+        <v>59</v>
+      </c>
+      <c r="D73" t="s">
+        <v>945</v>
+      </c>
+      <c r="E73">
+        <v>678</v>
+      </c>
+      <c r="F73">
+        <v>359</v>
+      </c>
+      <c r="J73">
+        <v>17</v>
+      </c>
+      <c r="K73">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11">
+      <c r="C74">
+        <v>60</v>
+      </c>
+      <c r="D74" t="s">
+        <v>946</v>
+      </c>
+      <c r="E74">
+        <v>727</v>
+      </c>
+      <c r="F74">
+        <v>360</v>
+      </c>
+      <c r="J74">
+        <v>17</v>
+      </c>
+      <c r="K74">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11">
+      <c r="C75">
+        <v>58</v>
+      </c>
+      <c r="D75" t="s">
+        <v>947</v>
+      </c>
+      <c r="E75">
+        <v>678</v>
+      </c>
+      <c r="F75">
+        <v>457</v>
+      </c>
+      <c r="J75">
+        <v>17</v>
+      </c>
+      <c r="K75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="3:11">
+      <c r="C76">
+        <v>61</v>
+      </c>
+      <c r="D76" t="s">
+        <v>948</v>
+      </c>
+      <c r="E76">
+        <v>727</v>
+      </c>
+      <c r="F76">
+        <v>456</v>
+      </c>
+      <c r="J76">
+        <v>17</v>
+      </c>
+      <c r="K76">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="3:11">
+      <c r="C77">
+        <v>57</v>
+      </c>
+      <c r="D77" t="s">
+        <v>949</v>
+      </c>
+      <c r="E77">
+        <v>680</v>
+      </c>
+      <c r="F77">
+        <v>540</v>
+      </c>
+      <c r="J77">
+        <v>17</v>
+      </c>
+      <c r="K77">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="3:11">
+      <c r="C78">
+        <v>62</v>
+      </c>
+      <c r="D78" t="s">
+        <v>950</v>
+      </c>
+      <c r="E78">
+        <v>725</v>
+      </c>
+      <c r="F78">
+        <v>537</v>
+      </c>
+      <c r="J78">
+        <v>17</v>
+      </c>
+      <c r="K78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="3:11">
+      <c r="C79">
+        <v>36</v>
+      </c>
+      <c r="D79" t="s">
+        <v>951</v>
+      </c>
+      <c r="E79">
+        <v>908</v>
+      </c>
+      <c r="F79">
+        <v>324</v>
+      </c>
+      <c r="J79">
+        <v>17</v>
+      </c>
+      <c r="K79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="3:11">
+      <c r="C80">
+        <v>35</v>
+      </c>
+      <c r="D80" t="s">
+        <v>952</v>
+      </c>
+      <c r="E80">
+        <v>909</v>
+      </c>
+      <c r="F80">
+        <v>409</v>
+      </c>
+      <c r="J80">
+        <v>17</v>
+      </c>
+      <c r="K80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="3:11">
+      <c r="C81">
+        <v>34</v>
+      </c>
+      <c r="D81" t="s">
+        <v>953</v>
+      </c>
+      <c r="E81">
+        <v>909</v>
+      </c>
+      <c r="F81">
+        <v>493</v>
+      </c>
+      <c r="J81">
+        <v>17</v>
+      </c>
+      <c r="K81">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="3:11">
+      <c r="C82">
+        <v>33</v>
+      </c>
+      <c r="D82" t="s">
+        <v>954</v>
+      </c>
+      <c r="E82">
+        <v>908</v>
+      </c>
+      <c r="F82">
+        <v>571</v>
+      </c>
+      <c r="J82">
+        <v>17</v>
+      </c>
+      <c r="K82">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="3:11">
+      <c r="C83">
+        <v>32</v>
+      </c>
+      <c r="D83" t="s">
+        <v>955</v>
+      </c>
+      <c r="E83">
+        <v>907</v>
+      </c>
+      <c r="F83">
+        <v>671</v>
+      </c>
+      <c r="J83">
+        <v>17</v>
+      </c>
+      <c r="K83">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="3:11">
+      <c r="C84">
+        <v>54</v>
+      </c>
+      <c r="D84" t="s">
+        <v>956</v>
+      </c>
+      <c r="E84">
+        <v>433</v>
+      </c>
+      <c r="F84">
+        <v>411</v>
+      </c>
+      <c r="J84">
+        <v>17</v>
+      </c>
+      <c r="K84">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="3:11">
+      <c r="C85">
+        <v>55</v>
+      </c>
+      <c r="D85" t="s">
+        <v>957</v>
+      </c>
+      <c r="E85">
+        <v>482</v>
+      </c>
+      <c r="F85">
+        <v>411</v>
+      </c>
+      <c r="J85">
+        <v>17</v>
+      </c>
+      <c r="K85">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="3:11">
+      <c r="C86">
+        <v>53</v>
+      </c>
+      <c r="D86" t="s">
+        <v>958</v>
+      </c>
+      <c r="E86">
+        <v>432</v>
+      </c>
+      <c r="F86">
+        <v>511</v>
+      </c>
+      <c r="J86">
+        <v>17</v>
+      </c>
+      <c r="K86">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="3:11">
+      <c r="C87">
+        <v>56</v>
+      </c>
+      <c r="D87" t="s">
+        <v>959</v>
+      </c>
+      <c r="E87">
+        <v>481</v>
+      </c>
+      <c r="F87">
+        <v>513</v>
+      </c>
+      <c r="J87">
+        <v>17</v>
+      </c>
+      <c r="K87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="3:11">
+      <c r="D89" t="s">
+        <v>799</v>
+      </c>
+      <c r="E89">
+        <v>956</v>
+      </c>
+      <c r="F89">
+        <v>39</v>
+      </c>
+      <c r="G89" t="s">
+        <v>800</v>
+      </c>
+      <c r="J89">
+        <v>74</v>
+      </c>
+      <c r="K89">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="3:11">
+      <c r="D90" t="s">
+        <v>801</v>
+      </c>
+      <c r="E90">
+        <v>52</v>
+      </c>
+      <c r="F90">
+        <v>80</v>
+      </c>
+      <c r="G90" t="s">
+        <v>802</v>
+      </c>
+      <c r="J90">
+        <v>74</v>
+      </c>
+      <c r="K90">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="3:11">
+      <c r="D92" t="s">
+        <v>803</v>
+      </c>
+      <c r="E92">
+        <v>65</v>
+      </c>
+      <c r="F92">
+        <v>839</v>
+      </c>
+      <c r="J92">
+        <v>65</v>
+      </c>
+      <c r="K92">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="3:11">
+      <c r="D93" t="s">
+        <v>804</v>
+      </c>
+      <c r="E93">
+        <v>269</v>
+      </c>
+      <c r="F93">
+        <v>838</v>
+      </c>
+      <c r="J93">
+        <v>65</v>
+      </c>
+      <c r="K93">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="3:11">
+      <c r="D94" t="s">
+        <v>805</v>
+      </c>
+      <c r="E94">
+        <v>559</v>
+      </c>
+      <c r="F94">
+        <v>857</v>
+      </c>
+      <c r="J94">
+        <v>65</v>
+      </c>
+      <c r="K94">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="3:11">
+      <c r="D95" t="s">
+        <v>806</v>
+      </c>
+      <c r="E95">
+        <v>988</v>
+      </c>
+      <c r="F95">
+        <v>754</v>
+      </c>
+      <c r="G95" t="s">
+        <v>807</v>
+      </c>
+      <c r="J95">
+        <v>74</v>
+      </c>
+      <c r="K95">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="3:11">
+      <c r="C97">
+        <v>10</v>
+      </c>
+      <c r="D97" t="s">
+        <v>960</v>
+      </c>
+      <c r="E97">
+        <v>248</v>
+      </c>
+      <c r="F97">
+        <v>947</v>
+      </c>
+      <c r="J97">
+        <v>65</v>
+      </c>
+      <c r="K97">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="3:11">
+      <c r="C98">
+        <v>11</v>
+      </c>
+      <c r="D98" t="s">
+        <v>961</v>
+      </c>
+      <c r="E98">
+        <v>23</v>
+      </c>
+      <c r="F98">
+        <v>923</v>
+      </c>
+      <c r="J98">
+        <v>65</v>
+      </c>
+      <c r="K98">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="3:11">
+      <c r="C99">
+        <v>15</v>
+      </c>
+      <c r="D99" t="s">
+        <v>962</v>
+      </c>
+      <c r="E99">
+        <v>595</v>
+      </c>
+      <c r="F99">
+        <v>921</v>
+      </c>
+      <c r="J99">
+        <v>65</v>
+      </c>
+      <c r="K99">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="3:11">
+      <c r="C100">
+        <v>12</v>
+      </c>
+      <c r="D100" t="s">
+        <v>963</v>
+      </c>
+      <c r="E100">
+        <v>183</v>
+      </c>
+      <c r="F100">
+        <v>1032</v>
+      </c>
+      <c r="J100">
+        <v>65</v>
+      </c>
+      <c r="K100">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="3:11">
+      <c r="C101">
+        <v>13</v>
+      </c>
+      <c r="D101" t="s">
+        <v>964</v>
+      </c>
+      <c r="E101">
+        <v>283</v>
+      </c>
+      <c r="F101">
+        <v>1035</v>
+      </c>
+      <c r="J101">
+        <v>65</v>
+      </c>
+      <c r="K101">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="3:11">
+      <c r="C102">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
+        <v>965</v>
+      </c>
+      <c r="E102">
+        <v>514</v>
+      </c>
+      <c r="F102">
+        <v>1036</v>
+      </c>
+      <c r="J102">
+        <v>65</v>
+      </c>
+      <c r="K102">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="3:11">
+      <c r="C103">
+        <v>16</v>
+      </c>
+      <c r="D103" t="s">
+        <v>966</v>
+      </c>
+      <c r="E103">
+        <v>625</v>
+      </c>
+      <c r="F103">
+        <v>1036</v>
+      </c>
+      <c r="J103">
+        <v>65</v>
+      </c>
+      <c r="K103">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="3:11">
+      <c r="D104" t="s">
+        <v>815</v>
+      </c>
+      <c r="E104">
+        <v>740</v>
+      </c>
+      <c r="F104">
+        <v>1038</v>
+      </c>
+      <c r="J104">
+        <v>65</v>
+      </c>
+      <c r="K104">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="3:11">
+      <c r="D105" t="s">
+        <v>816</v>
+      </c>
+      <c r="E105">
+        <v>851</v>
+      </c>
+      <c r="F105">
+        <v>918</v>
+      </c>
+      <c r="J105">
+        <v>65</v>
+      </c>
+      <c r="K105">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="3:11">
+      <c r="D106" t="s">
+        <v>817</v>
+      </c>
+      <c r="E106">
+        <v>845</v>
+      </c>
+      <c r="F106">
+        <v>1036</v>
+      </c>
+      <c r="J106">
+        <v>65</v>
+      </c>
+      <c r="K106">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="3:11">
+      <c r="D107" t="s">
+        <v>818</v>
+      </c>
+      <c r="E107">
+        <v>656</v>
+      </c>
+      <c r="F107">
+        <v>1099</v>
+      </c>
+      <c r="J107">
+        <v>65</v>
+      </c>
+      <c r="K107">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="3:11">
+      <c r="C109">
+        <v>25</v>
+      </c>
+      <c r="D109" t="s">
+        <v>967</v>
+      </c>
+      <c r="E109">
+        <v>233</v>
+      </c>
+      <c r="F109">
+        <v>1213</v>
+      </c>
+      <c r="G109" t="s">
+        <v>820</v>
+      </c>
+      <c r="J109">
+        <v>74</v>
+      </c>
+      <c r="K109">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="3:11">
+      <c r="C110">
+        <v>26</v>
+      </c>
+      <c r="D110" t="s">
+        <v>968</v>
+      </c>
+      <c r="E110">
+        <v>257</v>
+      </c>
+      <c r="F110">
+        <v>1051</v>
+      </c>
+      <c r="G110" t="s">
+        <v>822</v>
+      </c>
+      <c r="J110">
+        <v>74</v>
+      </c>
+      <c r="K110">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="3:11">
+      <c r="C111">
+        <v>22</v>
+      </c>
+      <c r="D111" t="s">
+        <v>969</v>
+      </c>
+      <c r="E111">
+        <v>829</v>
+      </c>
+      <c r="F111">
+        <v>1169</v>
+      </c>
+      <c r="G111" t="s">
+        <v>824</v>
+      </c>
+      <c r="J111">
+        <v>74</v>
+      </c>
+      <c r="K111">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="3:11">
+      <c r="C112" t="s">
+        <v>974</v>
+      </c>
+      <c r="D112" t="s">
+        <v>970</v>
+      </c>
+      <c r="E112">
+        <v>527</v>
+      </c>
+      <c r="F112">
+        <v>1186</v>
+      </c>
+      <c r="G112" t="s">
+        <v>826</v>
+      </c>
+      <c r="J112">
+        <v>74</v>
+      </c>
+      <c r="K112">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="3:11">
+      <c r="C113" t="s">
+        <v>975</v>
+      </c>
+      <c r="D113" t="s">
+        <v>971</v>
+      </c>
+      <c r="E113">
+        <v>460</v>
+      </c>
+      <c r="F113">
+        <v>1221</v>
+      </c>
+      <c r="G113" t="s">
+        <v>828</v>
+      </c>
+      <c r="J113">
+        <v>74</v>
+      </c>
+      <c r="K113">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="3:11">
+      <c r="C114">
+        <v>24</v>
+      </c>
+      <c r="D114" t="s">
+        <v>972</v>
+      </c>
+      <c r="E114">
+        <v>243</v>
+      </c>
+      <c r="F114">
+        <v>1335</v>
+      </c>
+      <c r="G114" t="s">
+        <v>830</v>
+      </c>
+      <c r="J114">
+        <v>74</v>
+      </c>
+      <c r="K114">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="3:11">
+      <c r="D115" t="s">
+        <v>831</v>
+      </c>
+      <c r="E115">
+        <v>799</v>
+      </c>
+      <c r="F115">
+        <v>1340</v>
+      </c>
+      <c r="G115" t="s">
+        <v>832</v>
+      </c>
+      <c r="J115">
+        <v>74</v>
+      </c>
+      <c r="K115">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="B161" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed a typo, about to finish updating scraped data input
</commit_message>
<xml_diff>
--- a/full-data-iday14.xlsx
+++ b/full-data-iday14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="2160" windowWidth="14360" windowHeight="17560" tabRatio="500" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="17560" tabRatio="500" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="current" sheetId="1" r:id="rId1"/>
@@ -4217,7 +4217,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="457">
+  <cellStyleXfs count="577">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4289,6 +4289,126 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5238,7 +5358,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="457">
+  <cellStyles count="577">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -5466,6 +5586,66 @@
     <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -5693,6 +5873,66 @@
     <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Output" xfId="70" builtinId="21"/>
@@ -6026,8 +6266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR105"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11276,7 +11516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AB149"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:I70"/>
     </sheetView>
   </sheetViews>
@@ -26312,7 +26552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X179"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="D36" workbookViewId="0">
       <selection activeCell="C58" sqref="C58:G119"/>
     </sheetView>
   </sheetViews>
@@ -28709,7 +28949,7 @@
   <dimension ref="A1:N108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N108"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>